<commit_message>
magnet Tabelle auf p=20 erweitert
</commit_message>
<xml_diff>
--- a/magnet.xlsx
+++ b/magnet.xlsx
@@ -5,17 +5,30 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kzt\Python_Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git-Repositories\Streamlit_Magnetgetriebe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2B3C2E-7E52-42DA-8A4E-E72BD5E369A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C21F9A-34ED-4233-A6A7-2BC259943DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F30568EE-B3B4-42DF-9CF1-B5E536E04381}"/>
   </bookViews>
   <sheets>
     <sheet name="test2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -878,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB0DFE6-30A2-4A15-91CE-18FDCD3EAF8D}">
-  <dimension ref="A1:AX31"/>
+  <dimension ref="A1:AX51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="A1:AX31"/>
+    <sheetView tabSelected="1" topLeftCell="AE28" workbookViewId="0">
+      <selection activeCell="AY42" sqref="AY42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5598,6 +5611,3046 @@
         <v>2.0369999999999999</v>
       </c>
     </row>
+    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>14</v>
+      </c>
+      <c r="B32" s="1">
+        <v>14</v>
+      </c>
+      <c r="C32" s="1">
+        <v>14</v>
+      </c>
+      <c r="D32" s="1">
+        <v>14</v>
+      </c>
+      <c r="E32" s="1">
+        <v>14</v>
+      </c>
+      <c r="F32" s="1">
+        <v>14</v>
+      </c>
+      <c r="G32" s="1">
+        <v>14</v>
+      </c>
+      <c r="H32" s="1">
+        <v>14</v>
+      </c>
+      <c r="I32" s="1">
+        <v>14</v>
+      </c>
+      <c r="J32" s="1">
+        <v>14</v>
+      </c>
+      <c r="K32" s="1">
+        <v>14</v>
+      </c>
+      <c r="L32" s="1">
+        <v>14</v>
+      </c>
+      <c r="M32" s="1">
+        <v>14</v>
+      </c>
+      <c r="N32" s="1">
+        <v>14</v>
+      </c>
+      <c r="O32" s="1">
+        <v>14</v>
+      </c>
+      <c r="P32" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>14</v>
+      </c>
+      <c r="R32" s="1">
+        <v>14</v>
+      </c>
+      <c r="S32" s="1">
+        <v>14</v>
+      </c>
+      <c r="T32" s="1">
+        <v>14</v>
+      </c>
+      <c r="U32" s="1">
+        <v>14</v>
+      </c>
+      <c r="V32" s="1">
+        <v>14</v>
+      </c>
+      <c r="W32" s="1">
+        <v>14</v>
+      </c>
+      <c r="X32" s="1">
+        <v>14</v>
+      </c>
+      <c r="Y32" s="1">
+        <v>14</v>
+      </c>
+      <c r="Z32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AA32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AB32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AC32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AD32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AE32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AF32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AG32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AH32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AI32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AJ32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AK32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AL32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AM32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AN32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AO32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AP32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AQ32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AR32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AS32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AT32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AU32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AV32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AW32" s="1">
+        <v>14</v>
+      </c>
+      <c r="AX32" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="B33">
+        <v>1.2857142857142856</v>
+      </c>
+      <c r="C33">
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="D33">
+        <v>1.5714285714285714</v>
+      </c>
+      <c r="E33">
+        <v>1.7142857142857144</v>
+      </c>
+      <c r="F33">
+        <v>1.8571428571428572</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="I33">
+        <v>2.2857142857142856</v>
+      </c>
+      <c r="J33">
+        <v>2.4285714285714288</v>
+      </c>
+      <c r="K33">
+        <v>2.5714285714285712</v>
+      </c>
+      <c r="L33">
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="M33">
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="N33">
+        <v>3</v>
+      </c>
+      <c r="O33">
+        <v>3.1428571428571428</v>
+      </c>
+      <c r="P33">
+        <v>3.2857142857142856</v>
+      </c>
+      <c r="Q33">
+        <v>3.4285714285714284</v>
+      </c>
+      <c r="R33">
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="S33">
+        <v>3.7142857142857144</v>
+      </c>
+      <c r="T33">
+        <v>3.8571428571428572</v>
+      </c>
+      <c r="U33">
+        <v>4</v>
+      </c>
+      <c r="V33">
+        <v>4.1428571428571423</v>
+      </c>
+      <c r="W33">
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="X33">
+        <v>4.4285714285714288</v>
+      </c>
+      <c r="Y33">
+        <v>4.5714285714285712</v>
+      </c>
+      <c r="Z33">
+        <v>4.7142857142857144</v>
+      </c>
+      <c r="AA33">
+        <v>4.8571428571428577</v>
+      </c>
+      <c r="AB33">
+        <v>5</v>
+      </c>
+      <c r="AC33">
+        <v>5.1428571428571432</v>
+      </c>
+      <c r="AD33">
+        <v>5.2857142857142856</v>
+      </c>
+      <c r="AE33">
+        <v>5.4285714285714288</v>
+      </c>
+      <c r="AF33">
+        <v>5.5714285714285712</v>
+      </c>
+      <c r="AG33">
+        <v>5.7142857142857144</v>
+      </c>
+      <c r="AH33">
+        <v>5.8571428571428568</v>
+      </c>
+      <c r="AI33">
+        <v>6</v>
+      </c>
+      <c r="AJ33">
+        <v>6.1428571428571432</v>
+      </c>
+      <c r="AK33">
+        <v>6.2857142857142856</v>
+      </c>
+      <c r="AL33">
+        <v>6.4285714285714288</v>
+      </c>
+      <c r="AM33">
+        <v>6.5714285714285712</v>
+      </c>
+      <c r="AN33">
+        <v>6.7142857142857144</v>
+      </c>
+      <c r="AO33">
+        <v>6.8571428571428568</v>
+      </c>
+      <c r="AP33">
+        <v>7</v>
+      </c>
+      <c r="AQ33">
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="AR33">
+        <v>7.2857142857142856</v>
+      </c>
+      <c r="AS33">
+        <v>7.4285714285714288</v>
+      </c>
+      <c r="AT33">
+        <v>7.5714285714285712</v>
+      </c>
+      <c r="AU33">
+        <v>7.7142857142857144</v>
+      </c>
+      <c r="AV33">
+        <v>7.8571428571428568</v>
+      </c>
+      <c r="AW33">
+        <v>8</v>
+      </c>
+      <c r="AX33">
+        <v>8.1428571428571423</v>
+      </c>
+    </row>
+    <row r="34" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>6.8550000000000004</v>
+      </c>
+      <c r="B34">
+        <v>17.55</v>
+      </c>
+      <c r="C34">
+        <v>24.427</v>
+      </c>
+      <c r="D34">
+        <v>31.541</v>
+      </c>
+      <c r="E34">
+        <v>34.264000000000003</v>
+      </c>
+      <c r="F34">
+        <v>36.984999999999999</v>
+      </c>
+      <c r="G34">
+        <v>25.550999999999998</v>
+      </c>
+      <c r="H34">
+        <v>38.777999999999999</v>
+      </c>
+      <c r="I34">
+        <v>38.061</v>
+      </c>
+      <c r="J34">
+        <v>37.593000000000004</v>
+      </c>
+      <c r="K34">
+        <v>37.298999999999999</v>
+      </c>
+      <c r="L34">
+        <v>37.563000000000002</v>
+      </c>
+      <c r="M34">
+        <v>36.406999999999996</v>
+      </c>
+      <c r="N34">
+        <v>37.578000000000003</v>
+      </c>
+      <c r="O34">
+        <v>37.390999999999998</v>
+      </c>
+      <c r="P34">
+        <v>36.863</v>
+      </c>
+      <c r="Q34">
+        <v>36.045000000000002</v>
+      </c>
+      <c r="R34">
+        <v>34.987000000000002</v>
+      </c>
+      <c r="S34">
+        <v>33.74</v>
+      </c>
+      <c r="T34">
+        <v>32.351999999999997</v>
+      </c>
+      <c r="U34">
+        <v>29.940999999999999</v>
+      </c>
+      <c r="V34">
+        <v>31.099</v>
+      </c>
+      <c r="W34">
+        <v>28.72</v>
+      </c>
+      <c r="X34">
+        <v>24.3</v>
+      </c>
+      <c r="Y34">
+        <v>21.920999999999999</v>
+      </c>
+      <c r="Z34">
+        <v>25.283999999999999</v>
+      </c>
+      <c r="AA34">
+        <v>28.646999999999998</v>
+      </c>
+      <c r="AB34">
+        <v>28.439</v>
+      </c>
+      <c r="AC34">
+        <v>27.9</v>
+      </c>
+      <c r="AD34">
+        <v>27.158999999999999</v>
+      </c>
+      <c r="AE34">
+        <v>26.344999999999999</v>
+      </c>
+      <c r="AF34">
+        <v>25.042999999999999</v>
+      </c>
+      <c r="AG34">
+        <v>23.23</v>
+      </c>
+      <c r="AH34">
+        <v>21.619</v>
+      </c>
+      <c r="AI34">
+        <v>20.922999999999998</v>
+      </c>
+      <c r="AJ34">
+        <v>23.452000000000002</v>
+      </c>
+      <c r="AK34">
+        <v>23.355</v>
+      </c>
+      <c r="AL34">
+        <v>23.088999999999999</v>
+      </c>
+      <c r="AM34">
+        <v>22.693999999999999</v>
+      </c>
+      <c r="AN34">
+        <v>22.209</v>
+      </c>
+      <c r="AO34">
+        <v>21.672999999999998</v>
+      </c>
+      <c r="AP34">
+        <v>21.125</v>
+      </c>
+      <c r="AQ34">
+        <v>20.605</v>
+      </c>
+      <c r="AR34">
+        <v>20.027999999999999</v>
+      </c>
+      <c r="AS34">
+        <v>19.36</v>
+      </c>
+      <c r="AT34">
+        <v>18.713999999999999</v>
+      </c>
+      <c r="AU34">
+        <v>18.202999999999999</v>
+      </c>
+      <c r="AV34">
+        <v>17.821000000000002</v>
+      </c>
+      <c r="AW34">
+        <v>17.5</v>
+      </c>
+      <c r="AX34">
+        <v>17.260999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="B35">
+        <v>4.0229999999999997</v>
+      </c>
+      <c r="C35">
+        <v>7.1710000000000003</v>
+      </c>
+      <c r="D35">
+        <v>11.113</v>
+      </c>
+      <c r="E35">
+        <v>14.239000000000001</v>
+      </c>
+      <c r="F35">
+        <v>16.637</v>
+      </c>
+      <c r="G35">
+        <v>10.920999999999999</v>
+      </c>
+      <c r="H35">
+        <v>20.013000000000002</v>
+      </c>
+      <c r="I35">
+        <v>22.559000000000001</v>
+      </c>
+      <c r="J35">
+        <v>23.472999999999999</v>
+      </c>
+      <c r="K35">
+        <v>23.065999999999999</v>
+      </c>
+      <c r="L35">
+        <v>24.228999999999999</v>
+      </c>
+      <c r="M35">
+        <v>24.739000000000001</v>
+      </c>
+      <c r="N35">
+        <v>25.795999999999999</v>
+      </c>
+      <c r="O35">
+        <v>25.751000000000001</v>
+      </c>
+      <c r="P35">
+        <v>25.606000000000002</v>
+      </c>
+      <c r="Q35">
+        <v>25.347000000000001</v>
+      </c>
+      <c r="R35">
+        <v>24.957000000000001</v>
+      </c>
+      <c r="S35">
+        <v>24.422999999999998</v>
+      </c>
+      <c r="T35">
+        <v>23.728999999999999</v>
+      </c>
+      <c r="U35">
+        <v>20.245000000000001</v>
+      </c>
+      <c r="V35">
+        <v>22.49</v>
+      </c>
+      <c r="W35">
+        <v>22.405999999999999</v>
+      </c>
+      <c r="X35">
+        <v>22.195</v>
+      </c>
+      <c r="Y35">
+        <v>21.920999999999999</v>
+      </c>
+      <c r="Z35">
+        <v>21.443999999999999</v>
+      </c>
+      <c r="AA35">
+        <v>20.9</v>
+      </c>
+      <c r="AB35">
+        <v>20.503</v>
+      </c>
+      <c r="AC35">
+        <v>20.145</v>
+      </c>
+      <c r="AD35">
+        <v>19.824000000000002</v>
+      </c>
+      <c r="AE35">
+        <v>19.533999999999999</v>
+      </c>
+      <c r="AF35">
+        <v>19.236000000000001</v>
+      </c>
+      <c r="AG35">
+        <v>18.937000000000001</v>
+      </c>
+      <c r="AH35">
+        <v>18.706</v>
+      </c>
+      <c r="AI35">
+        <v>18.614000000000001</v>
+      </c>
+      <c r="AJ35">
+        <v>22.16</v>
+      </c>
+      <c r="AK35">
+        <v>21.757000000000001</v>
+      </c>
+      <c r="AL35">
+        <v>20.719000000000001</v>
+      </c>
+      <c r="AM35">
+        <v>19.297999999999998</v>
+      </c>
+      <c r="AN35">
+        <v>17.751000000000001</v>
+      </c>
+      <c r="AO35">
+        <v>16.329999999999998</v>
+      </c>
+      <c r="AP35">
+        <v>15.292</v>
+      </c>
+      <c r="AQ35">
+        <v>14.888999999999999</v>
+      </c>
+      <c r="AR35">
+        <v>15.613</v>
+      </c>
+      <c r="AS35">
+        <v>17.207000000000001</v>
+      </c>
+      <c r="AT35">
+        <v>18.800999999999998</v>
+      </c>
+      <c r="AU35">
+        <v>19.524999999999999</v>
+      </c>
+      <c r="AV35">
+        <v>19.446999999999999</v>
+      </c>
+      <c r="AW35">
+        <v>19.097000000000001</v>
+      </c>
+      <c r="AX35">
+        <v>18.298999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>6.5289999999999999</v>
+      </c>
+      <c r="B36">
+        <v>13.34</v>
+      </c>
+      <c r="C36">
+        <v>17.780999999999999</v>
+      </c>
+      <c r="D36">
+        <v>20.032</v>
+      </c>
+      <c r="E36">
+        <v>20.594000000000001</v>
+      </c>
+      <c r="F36">
+        <v>19.977</v>
+      </c>
+      <c r="G36">
+        <v>14.78</v>
+      </c>
+      <c r="H36">
+        <v>17.832999999999998</v>
+      </c>
+      <c r="I36">
+        <v>16.826000000000001</v>
+      </c>
+      <c r="J36">
+        <v>15.749000000000001</v>
+      </c>
+      <c r="K36">
+        <v>14.616</v>
+      </c>
+      <c r="L36">
+        <v>13.769</v>
+      </c>
+      <c r="M36">
+        <v>13.105</v>
+      </c>
+      <c r="N36">
+        <v>13.547000000000001</v>
+      </c>
+      <c r="O36">
+        <v>13.175000000000001</v>
+      </c>
+      <c r="P36">
+        <v>12.247</v>
+      </c>
+      <c r="Q36">
+        <v>11.039</v>
+      </c>
+      <c r="R36">
+        <v>9.8309999999999995</v>
+      </c>
+      <c r="S36">
+        <v>8.9019999999999992</v>
+      </c>
+      <c r="T36">
+        <v>8.5310000000000006</v>
+      </c>
+      <c r="U36">
+        <v>8.5470000000000006</v>
+      </c>
+      <c r="V36">
+        <v>7.6619999999999999</v>
+      </c>
+      <c r="W36">
+        <v>7.2130000000000001</v>
+      </c>
+      <c r="X36">
+        <v>6.89</v>
+      </c>
+      <c r="Y36">
+        <v>6.5819999999999999</v>
+      </c>
+      <c r="Z36">
+        <v>6.2480000000000002</v>
+      </c>
+      <c r="AA36">
+        <v>5.9370000000000003</v>
+      </c>
+      <c r="AB36">
+        <v>5.609</v>
+      </c>
+      <c r="AC36">
+        <v>5.2679999999999998</v>
+      </c>
+      <c r="AD36">
+        <v>5</v>
+      </c>
+      <c r="AE36">
+        <v>4.8920000000000003</v>
+      </c>
+      <c r="AF36">
+        <v>4.9779999999999998</v>
+      </c>
+      <c r="AG36">
+        <v>5.1689999999999996</v>
+      </c>
+      <c r="AH36">
+        <v>5.36</v>
+      </c>
+      <c r="AI36">
+        <v>5.4459999999999997</v>
+      </c>
+      <c r="AJ36">
+        <v>3.9140000000000001</v>
+      </c>
+      <c r="AK36">
+        <v>3.6280000000000001</v>
+      </c>
+      <c r="AL36">
+        <v>3.4209999999999998</v>
+      </c>
+      <c r="AM36">
+        <v>3.2719999999999998</v>
+      </c>
+      <c r="AN36">
+        <v>3.1659999999999999</v>
+      </c>
+      <c r="AO36">
+        <v>3.0819999999999999</v>
+      </c>
+      <c r="AP36">
+        <v>3.0030000000000001</v>
+      </c>
+      <c r="AQ36">
+        <v>2.911</v>
+      </c>
+      <c r="AR36">
+        <v>2.8170000000000002</v>
+      </c>
+      <c r="AS36">
+        <v>2.7360000000000002</v>
+      </c>
+      <c r="AT36">
+        <v>2.657</v>
+      </c>
+      <c r="AU36">
+        <v>2.5670000000000002</v>
+      </c>
+      <c r="AV36">
+        <v>2.46</v>
+      </c>
+      <c r="AW36">
+        <v>2.3410000000000002</v>
+      </c>
+      <c r="AX36">
+        <v>2.2130000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>16</v>
+      </c>
+      <c r="B37">
+        <v>16</v>
+      </c>
+      <c r="C37">
+        <v>16</v>
+      </c>
+      <c r="D37">
+        <v>16</v>
+      </c>
+      <c r="E37">
+        <v>16</v>
+      </c>
+      <c r="F37">
+        <v>16</v>
+      </c>
+      <c r="G37">
+        <v>16</v>
+      </c>
+      <c r="H37">
+        <v>16</v>
+      </c>
+      <c r="I37">
+        <v>16</v>
+      </c>
+      <c r="J37">
+        <v>16</v>
+      </c>
+      <c r="K37">
+        <v>16</v>
+      </c>
+      <c r="L37">
+        <v>16</v>
+      </c>
+      <c r="M37">
+        <v>16</v>
+      </c>
+      <c r="N37">
+        <v>16</v>
+      </c>
+      <c r="O37">
+        <v>16</v>
+      </c>
+      <c r="P37">
+        <v>16</v>
+      </c>
+      <c r="Q37">
+        <v>16</v>
+      </c>
+      <c r="R37">
+        <v>16</v>
+      </c>
+      <c r="S37">
+        <v>16</v>
+      </c>
+      <c r="T37">
+        <v>16</v>
+      </c>
+      <c r="U37">
+        <v>16</v>
+      </c>
+      <c r="V37">
+        <v>16</v>
+      </c>
+      <c r="W37">
+        <v>16</v>
+      </c>
+      <c r="X37">
+        <v>16</v>
+      </c>
+      <c r="Y37">
+        <v>16</v>
+      </c>
+      <c r="Z37">
+        <v>16</v>
+      </c>
+      <c r="AA37">
+        <v>16</v>
+      </c>
+      <c r="AB37">
+        <v>16</v>
+      </c>
+      <c r="AC37">
+        <v>16</v>
+      </c>
+      <c r="AD37">
+        <v>16</v>
+      </c>
+      <c r="AE37">
+        <v>16</v>
+      </c>
+      <c r="AF37">
+        <v>16</v>
+      </c>
+      <c r="AG37">
+        <v>16</v>
+      </c>
+      <c r="AH37">
+        <v>16</v>
+      </c>
+      <c r="AI37">
+        <v>16</v>
+      </c>
+      <c r="AJ37">
+        <v>16</v>
+      </c>
+      <c r="AK37">
+        <v>16</v>
+      </c>
+      <c r="AL37">
+        <v>16</v>
+      </c>
+      <c r="AM37">
+        <v>16</v>
+      </c>
+      <c r="AN37">
+        <v>16</v>
+      </c>
+      <c r="AO37">
+        <v>16</v>
+      </c>
+      <c r="AP37">
+        <v>16</v>
+      </c>
+      <c r="AQ37">
+        <v>16</v>
+      </c>
+      <c r="AR37">
+        <v>16</v>
+      </c>
+      <c r="AS37">
+        <v>16</v>
+      </c>
+      <c r="AT37">
+        <v>16</v>
+      </c>
+      <c r="AU37">
+        <v>16</v>
+      </c>
+      <c r="AV37">
+        <v>16</v>
+      </c>
+      <c r="AW37">
+        <v>16</v>
+      </c>
+      <c r="AX37">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1.125</v>
+      </c>
+      <c r="B38">
+        <v>1.25</v>
+      </c>
+      <c r="C38">
+        <v>1.375</v>
+      </c>
+      <c r="D38">
+        <v>1.5</v>
+      </c>
+      <c r="E38">
+        <v>1.625</v>
+      </c>
+      <c r="F38">
+        <v>1.75</v>
+      </c>
+      <c r="G38">
+        <v>1.875</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>2.125</v>
+      </c>
+      <c r="J38">
+        <v>2.25</v>
+      </c>
+      <c r="K38">
+        <v>2.375</v>
+      </c>
+      <c r="L38">
+        <v>2.5</v>
+      </c>
+      <c r="M38">
+        <v>2.625</v>
+      </c>
+      <c r="N38">
+        <v>2.75</v>
+      </c>
+      <c r="O38">
+        <v>2.875</v>
+      </c>
+      <c r="P38">
+        <v>3</v>
+      </c>
+      <c r="Q38">
+        <v>3.125</v>
+      </c>
+      <c r="R38">
+        <v>3.25</v>
+      </c>
+      <c r="S38">
+        <v>3.375</v>
+      </c>
+      <c r="T38">
+        <v>3.5</v>
+      </c>
+      <c r="U38">
+        <v>3.625</v>
+      </c>
+      <c r="V38">
+        <v>3.75</v>
+      </c>
+      <c r="W38">
+        <v>3.875</v>
+      </c>
+      <c r="X38">
+        <v>4</v>
+      </c>
+      <c r="Y38">
+        <v>4.125</v>
+      </c>
+      <c r="Z38">
+        <v>4.25</v>
+      </c>
+      <c r="AA38">
+        <v>4.375</v>
+      </c>
+      <c r="AB38">
+        <v>4.5</v>
+      </c>
+      <c r="AC38">
+        <v>4.625</v>
+      </c>
+      <c r="AD38">
+        <v>4.75</v>
+      </c>
+      <c r="AE38">
+        <v>4.875</v>
+      </c>
+      <c r="AF38">
+        <v>5</v>
+      </c>
+      <c r="AG38">
+        <v>5.125</v>
+      </c>
+      <c r="AH38">
+        <v>5.25</v>
+      </c>
+      <c r="AI38">
+        <v>5.375</v>
+      </c>
+      <c r="AJ38">
+        <v>5.5</v>
+      </c>
+      <c r="AK38">
+        <v>5.625</v>
+      </c>
+      <c r="AL38">
+        <v>5.75</v>
+      </c>
+      <c r="AM38">
+        <v>5.875</v>
+      </c>
+      <c r="AN38">
+        <v>6</v>
+      </c>
+      <c r="AO38">
+        <v>6.125</v>
+      </c>
+      <c r="AP38">
+        <v>6.25</v>
+      </c>
+      <c r="AQ38">
+        <v>6.375</v>
+      </c>
+      <c r="AR38">
+        <v>6.5</v>
+      </c>
+      <c r="AS38">
+        <v>6.625</v>
+      </c>
+      <c r="AT38">
+        <v>6.75</v>
+      </c>
+      <c r="AU38">
+        <v>6.875</v>
+      </c>
+      <c r="AV38">
+        <v>7</v>
+      </c>
+      <c r="AW38">
+        <v>7.125</v>
+      </c>
+      <c r="AX38">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>6.8819999999999997</v>
+      </c>
+      <c r="B39">
+        <v>18.625</v>
+      </c>
+      <c r="C39">
+        <v>26.263999999999999</v>
+      </c>
+      <c r="D39">
+        <v>34.796999999999997</v>
+      </c>
+      <c r="E39">
+        <v>35.384</v>
+      </c>
+      <c r="F39">
+        <v>36.887999999999998</v>
+      </c>
+      <c r="G39">
+        <v>37.512</v>
+      </c>
+      <c r="H39">
+        <v>28.463000000000001</v>
+      </c>
+      <c r="I39">
+        <v>38.103999999999999</v>
+      </c>
+      <c r="J39">
+        <v>37.331000000000003</v>
+      </c>
+      <c r="K39">
+        <v>36.798999999999999</v>
+      </c>
+      <c r="L39">
+        <v>37.634</v>
+      </c>
+      <c r="M39">
+        <v>36.225999999999999</v>
+      </c>
+      <c r="N39">
+        <v>35.076999999999998</v>
+      </c>
+      <c r="O39">
+        <v>34.304000000000002</v>
+      </c>
+      <c r="P39">
+        <v>33.649000000000001</v>
+      </c>
+      <c r="Q39">
+        <v>33.079000000000001</v>
+      </c>
+      <c r="R39">
+        <v>32.561</v>
+      </c>
+      <c r="S39">
+        <v>32.061999999999998</v>
+      </c>
+      <c r="T39">
+        <v>31.547000000000001</v>
+      </c>
+      <c r="U39">
+        <v>30.984000000000002</v>
+      </c>
+      <c r="V39">
+        <v>30.373000000000001</v>
+      </c>
+      <c r="W39">
+        <v>29.745999999999999</v>
+      </c>
+      <c r="X39">
+        <v>29.113</v>
+      </c>
+      <c r="Y39">
+        <v>28.489000000000001</v>
+      </c>
+      <c r="Z39">
+        <v>27.884</v>
+      </c>
+      <c r="AA39">
+        <v>27.31</v>
+      </c>
+      <c r="AB39">
+        <v>26.797999999999998</v>
+      </c>
+      <c r="AC39">
+        <v>26.350999999999999</v>
+      </c>
+      <c r="AD39">
+        <v>25.937000000000001</v>
+      </c>
+      <c r="AE39">
+        <v>25.526</v>
+      </c>
+      <c r="AF39">
+        <v>25.087</v>
+      </c>
+      <c r="AG39">
+        <v>24.59</v>
+      </c>
+      <c r="AH39">
+        <v>24.004999999999999</v>
+      </c>
+      <c r="AI39">
+        <v>23.3</v>
+      </c>
+      <c r="AJ39">
+        <v>22.16</v>
+      </c>
+      <c r="AK39">
+        <v>21.483000000000001</v>
+      </c>
+      <c r="AL39">
+        <v>20.917999999999999</v>
+      </c>
+      <c r="AM39">
+        <v>20.440000000000001</v>
+      </c>
+      <c r="AN39">
+        <v>20.023</v>
+      </c>
+      <c r="AO39">
+        <v>19.64</v>
+      </c>
+      <c r="AP39">
+        <v>19.265000000000001</v>
+      </c>
+      <c r="AQ39">
+        <v>18.870999999999999</v>
+      </c>
+      <c r="AR39">
+        <v>18.465</v>
+      </c>
+      <c r="AS39">
+        <v>18.071000000000002</v>
+      </c>
+      <c r="AT39">
+        <v>17.690000000000001</v>
+      </c>
+      <c r="AU39">
+        <v>17.321999999999999</v>
+      </c>
+      <c r="AV39">
+        <v>16.969000000000001</v>
+      </c>
+      <c r="AW39">
+        <v>16.63</v>
+      </c>
+      <c r="AX39">
+        <v>16.308</v>
+      </c>
+    </row>
+    <row r="40" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0.75</v>
+      </c>
+      <c r="B40">
+        <v>4.4240000000000004</v>
+      </c>
+      <c r="C40">
+        <v>7.01</v>
+      </c>
+      <c r="D40">
+        <v>13.365</v>
+      </c>
+      <c r="E40">
+        <v>13.618</v>
+      </c>
+      <c r="F40">
+        <v>15.457000000000001</v>
+      </c>
+      <c r="G40">
+        <v>17.771999999999998</v>
+      </c>
+      <c r="H40">
+        <v>11.872999999999999</v>
+      </c>
+      <c r="I40">
+        <v>19.634</v>
+      </c>
+      <c r="J40">
+        <v>21.734999999999999</v>
+      </c>
+      <c r="K40">
+        <v>21.488</v>
+      </c>
+      <c r="L40">
+        <v>21.446000000000002</v>
+      </c>
+      <c r="M40">
+        <v>22.018999999999998</v>
+      </c>
+      <c r="N40">
+        <v>22.594000000000001</v>
+      </c>
+      <c r="O40">
+        <v>22.568999999999999</v>
+      </c>
+      <c r="P40">
+        <v>22.5</v>
+      </c>
+      <c r="Q40">
+        <v>22.395</v>
+      </c>
+      <c r="R40">
+        <v>22.259</v>
+      </c>
+      <c r="S40">
+        <v>22.102</v>
+      </c>
+      <c r="T40">
+        <v>21.93</v>
+      </c>
+      <c r="U40">
+        <v>21.751000000000001</v>
+      </c>
+      <c r="V40">
+        <v>21.523</v>
+      </c>
+      <c r="W40">
+        <v>21.215</v>
+      </c>
+      <c r="X40">
+        <v>20.853000000000002</v>
+      </c>
+      <c r="Y40">
+        <v>20.463999999999999</v>
+      </c>
+      <c r="Z40">
+        <v>20.073</v>
+      </c>
+      <c r="AA40">
+        <v>19.704999999999998</v>
+      </c>
+      <c r="AB40">
+        <v>19.318000000000001</v>
+      </c>
+      <c r="AC40">
+        <v>18.872</v>
+      </c>
+      <c r="AD40">
+        <v>18.402000000000001</v>
+      </c>
+      <c r="AE40">
+        <v>17.942</v>
+      </c>
+      <c r="AF40">
+        <v>17.524999999999999</v>
+      </c>
+      <c r="AG40">
+        <v>17.184999999999999</v>
+      </c>
+      <c r="AH40">
+        <v>16.957000000000001</v>
+      </c>
+      <c r="AI40">
+        <v>16.873000000000001</v>
+      </c>
+      <c r="AJ40">
+        <v>21</v>
+      </c>
+      <c r="AK40">
+        <v>20.975999999999999</v>
+      </c>
+      <c r="AL40">
+        <v>20.908999999999999</v>
+      </c>
+      <c r="AM40">
+        <v>20.806000000000001</v>
+      </c>
+      <c r="AN40">
+        <v>20.672999999999998</v>
+      </c>
+      <c r="AO40">
+        <v>20.515000000000001</v>
+      </c>
+      <c r="AP40">
+        <v>20.341000000000001</v>
+      </c>
+      <c r="AQ40">
+        <v>20.155999999999999</v>
+      </c>
+      <c r="AR40">
+        <v>19.922999999999998</v>
+      </c>
+      <c r="AS40">
+        <v>19.606999999999999</v>
+      </c>
+      <c r="AT40">
+        <v>19.219000000000001</v>
+      </c>
+      <c r="AU40">
+        <v>18.77</v>
+      </c>
+      <c r="AV40">
+        <v>18.268999999999998</v>
+      </c>
+      <c r="AW40">
+        <v>17.728000000000002</v>
+      </c>
+      <c r="AX40">
+        <v>17.157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>6.085</v>
+      </c>
+      <c r="B41">
+        <v>14.343999999999999</v>
+      </c>
+      <c r="C41">
+        <v>18.925999999999998</v>
+      </c>
+      <c r="D41">
+        <v>22.108000000000001</v>
+      </c>
+      <c r="E41">
+        <v>21.632999999999999</v>
+      </c>
+      <c r="F41">
+        <v>21.091999999999999</v>
+      </c>
+      <c r="G41">
+        <v>20.126999999999999</v>
+      </c>
+      <c r="H41">
+        <v>15.875999999999999</v>
+      </c>
+      <c r="I41">
+        <v>17.867999999999999</v>
+      </c>
+      <c r="J41">
+        <v>16.754000000000001</v>
+      </c>
+      <c r="K41">
+        <v>15.785</v>
+      </c>
+      <c r="L41">
+        <v>14.829000000000001</v>
+      </c>
+      <c r="M41">
+        <v>13.891999999999999</v>
+      </c>
+      <c r="N41">
+        <v>13.058999999999999</v>
+      </c>
+      <c r="O41">
+        <v>12.318</v>
+      </c>
+      <c r="P41">
+        <v>11.598000000000001</v>
+      </c>
+      <c r="Q41">
+        <v>10.906000000000001</v>
+      </c>
+      <c r="R41">
+        <v>10.25</v>
+      </c>
+      <c r="S41">
+        <v>9.6379999999999999</v>
+      </c>
+      <c r="T41">
+        <v>9.0779999999999994</v>
+      </c>
+      <c r="U41">
+        <v>8.5779999999999994</v>
+      </c>
+      <c r="V41">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="W41">
+        <v>7.7160000000000002</v>
+      </c>
+      <c r="X41">
+        <v>7.335</v>
+      </c>
+      <c r="Y41">
+        <v>6.9820000000000002</v>
+      </c>
+      <c r="Z41">
+        <v>6.6539999999999999</v>
+      </c>
+      <c r="AA41">
+        <v>6.3460000000000001</v>
+      </c>
+      <c r="AB41">
+        <v>6.0579999999999998</v>
+      </c>
+      <c r="AC41">
+        <v>5.7889999999999997</v>
+      </c>
+      <c r="AD41">
+        <v>5.5339999999999998</v>
+      </c>
+      <c r="AE41">
+        <v>5.2919999999999998</v>
+      </c>
+      <c r="AF41">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="AG41">
+        <v>4.8339999999999996</v>
+      </c>
+      <c r="AH41">
+        <v>4.6120000000000001</v>
+      </c>
+      <c r="AI41">
+        <v>4.391</v>
+      </c>
+      <c r="AJ41">
+        <v>4.181</v>
+      </c>
+      <c r="AK41">
+        <v>3.996</v>
+      </c>
+      <c r="AL41">
+        <v>3.819</v>
+      </c>
+      <c r="AM41">
+        <v>3.649</v>
+      </c>
+      <c r="AN41">
+        <v>3.488</v>
+      </c>
+      <c r="AO41">
+        <v>3.3370000000000002</v>
+      </c>
+      <c r="AP41">
+        <v>3.1960000000000002</v>
+      </c>
+      <c r="AQ41">
+        <v>3.0670000000000002</v>
+      </c>
+      <c r="AR41">
+        <v>2.9470000000000001</v>
+      </c>
+      <c r="AS41">
+        <v>2.8319999999999999</v>
+      </c>
+      <c r="AT41">
+        <v>2.7240000000000002</v>
+      </c>
+      <c r="AU41">
+        <v>2.6219999999999999</v>
+      </c>
+      <c r="AV41">
+        <v>2.528</v>
+      </c>
+      <c r="AW41">
+        <v>2.4430000000000001</v>
+      </c>
+      <c r="AX41">
+        <v>2.3679999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>18</v>
+      </c>
+      <c r="B42">
+        <v>18</v>
+      </c>
+      <c r="C42">
+        <v>18</v>
+      </c>
+      <c r="D42">
+        <v>18</v>
+      </c>
+      <c r="E42">
+        <v>18</v>
+      </c>
+      <c r="F42">
+        <v>18</v>
+      </c>
+      <c r="G42">
+        <v>18</v>
+      </c>
+      <c r="H42">
+        <v>18</v>
+      </c>
+      <c r="I42">
+        <v>18</v>
+      </c>
+      <c r="J42">
+        <v>18</v>
+      </c>
+      <c r="K42">
+        <v>18</v>
+      </c>
+      <c r="L42">
+        <v>18</v>
+      </c>
+      <c r="M42">
+        <v>18</v>
+      </c>
+      <c r="N42">
+        <v>18</v>
+      </c>
+      <c r="O42">
+        <v>18</v>
+      </c>
+      <c r="P42">
+        <v>18</v>
+      </c>
+      <c r="Q42">
+        <v>18</v>
+      </c>
+      <c r="R42">
+        <v>18</v>
+      </c>
+      <c r="S42">
+        <v>18</v>
+      </c>
+      <c r="T42">
+        <v>18</v>
+      </c>
+      <c r="U42">
+        <v>18</v>
+      </c>
+      <c r="V42">
+        <v>18</v>
+      </c>
+      <c r="W42">
+        <v>18</v>
+      </c>
+      <c r="X42">
+        <v>18</v>
+      </c>
+      <c r="Y42">
+        <v>18</v>
+      </c>
+      <c r="Z42">
+        <v>18</v>
+      </c>
+      <c r="AA42">
+        <v>18</v>
+      </c>
+      <c r="AB42">
+        <v>18</v>
+      </c>
+      <c r="AC42">
+        <v>18</v>
+      </c>
+      <c r="AD42">
+        <v>18</v>
+      </c>
+      <c r="AE42">
+        <v>18</v>
+      </c>
+      <c r="AF42">
+        <v>18</v>
+      </c>
+      <c r="AG42">
+        <v>18</v>
+      </c>
+      <c r="AH42">
+        <v>18</v>
+      </c>
+      <c r="AI42">
+        <v>18</v>
+      </c>
+      <c r="AJ42">
+        <v>18</v>
+      </c>
+      <c r="AK42">
+        <v>18</v>
+      </c>
+      <c r="AL42">
+        <v>18</v>
+      </c>
+      <c r="AM42">
+        <v>18</v>
+      </c>
+      <c r="AN42">
+        <v>18</v>
+      </c>
+      <c r="AO42">
+        <v>18</v>
+      </c>
+      <c r="AP42">
+        <v>18</v>
+      </c>
+      <c r="AQ42">
+        <v>18</v>
+      </c>
+      <c r="AR42">
+        <v>18</v>
+      </c>
+      <c r="AS42">
+        <v>18</v>
+      </c>
+      <c r="AT42">
+        <v>18</v>
+      </c>
+      <c r="AU42">
+        <v>18</v>
+      </c>
+      <c r="AV42">
+        <v>18</v>
+      </c>
+      <c r="AW42">
+        <v>18</v>
+      </c>
+      <c r="AX42">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="B43">
+        <v>1.2222222222222223</v>
+      </c>
+      <c r="C43">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="D43">
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="E43">
+        <v>1.5555555555555556</v>
+      </c>
+      <c r="F43">
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="G43">
+        <v>1.7777777777777777</v>
+      </c>
+      <c r="H43">
+        <v>1.8888888888888888</v>
+      </c>
+      <c r="I43">
+        <v>2</v>
+      </c>
+      <c r="J43">
+        <v>2.1111111111111112</v>
+      </c>
+      <c r="K43">
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="L43">
+        <v>2.333333333333333</v>
+      </c>
+      <c r="M43">
+        <v>2.4444444444444446</v>
+      </c>
+      <c r="N43">
+        <v>2.5555555555555554</v>
+      </c>
+      <c r="O43">
+        <v>2.666666666666667</v>
+      </c>
+      <c r="P43">
+        <v>2.7777777777777777</v>
+      </c>
+      <c r="Q43">
+        <v>2.8888888888888888</v>
+      </c>
+      <c r="R43">
+        <v>3</v>
+      </c>
+      <c r="S43">
+        <v>3.1111111111111112</v>
+      </c>
+      <c r="T43">
+        <v>3.2222222222222223</v>
+      </c>
+      <c r="U43">
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="V43">
+        <v>3.4444444444444446</v>
+      </c>
+      <c r="W43">
+        <v>3.5555555555555554</v>
+      </c>
+      <c r="X43">
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="Y43">
+        <v>3.7777777777777777</v>
+      </c>
+      <c r="Z43">
+        <v>3.8888888888888888</v>
+      </c>
+      <c r="AA43">
+        <v>4</v>
+      </c>
+      <c r="AB43">
+        <v>4.1111111111111107</v>
+      </c>
+      <c r="AC43">
+        <v>4.2222222222222223</v>
+      </c>
+      <c r="AD43">
+        <v>4.3333333333333339</v>
+      </c>
+      <c r="AE43">
+        <v>4.4444444444444446</v>
+      </c>
+      <c r="AF43">
+        <v>4.5555555555555554</v>
+      </c>
+      <c r="AG43">
+        <v>4.6666666666666661</v>
+      </c>
+      <c r="AH43">
+        <v>4.7777777777777777</v>
+      </c>
+      <c r="AI43">
+        <v>4.8888888888888893</v>
+      </c>
+      <c r="AJ43">
+        <v>5</v>
+      </c>
+      <c r="AK43">
+        <v>5.1111111111111107</v>
+      </c>
+      <c r="AL43">
+        <v>5.2222222222222223</v>
+      </c>
+      <c r="AM43">
+        <v>5.333333333333333</v>
+      </c>
+      <c r="AN43">
+        <v>5.4444444444444446</v>
+      </c>
+      <c r="AO43">
+        <v>5.5555555555555554</v>
+      </c>
+      <c r="AP43">
+        <v>5.666666666666667</v>
+      </c>
+      <c r="AQ43">
+        <v>5.7777777777777777</v>
+      </c>
+      <c r="AR43">
+        <v>5.8888888888888893</v>
+      </c>
+      <c r="AS43">
+        <v>6</v>
+      </c>
+      <c r="AT43">
+        <v>6.1111111111111107</v>
+      </c>
+      <c r="AU43">
+        <v>6.2222222222222223</v>
+      </c>
+      <c r="AV43">
+        <v>6.333333333333333</v>
+      </c>
+      <c r="AW43">
+        <v>6.4444444444444446</v>
+      </c>
+      <c r="AX43">
+        <v>6.5555555555555554</v>
+      </c>
+    </row>
+    <row r="44" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>7.024</v>
+      </c>
+      <c r="B44">
+        <v>17.890999999999998</v>
+      </c>
+      <c r="C44">
+        <v>20.375</v>
+      </c>
+      <c r="D44">
+        <v>31.635000000000002</v>
+      </c>
+      <c r="E44">
+        <v>34.787999999999997</v>
+      </c>
+      <c r="F44">
+        <v>36.567</v>
+      </c>
+      <c r="G44">
+        <v>37.472000000000001</v>
+      </c>
+      <c r="H44">
+        <v>37.548000000000002</v>
+      </c>
+      <c r="I44">
+        <v>30.902999999999999</v>
+      </c>
+      <c r="J44">
+        <v>37.173000000000002</v>
+      </c>
+      <c r="K44">
+        <v>36.15</v>
+      </c>
+      <c r="L44">
+        <v>36.21</v>
+      </c>
+      <c r="M44">
+        <v>34.792000000000002</v>
+      </c>
+      <c r="N44">
+        <v>34.313000000000002</v>
+      </c>
+      <c r="O44">
+        <v>33.750999999999998</v>
+      </c>
+      <c r="P44">
+        <v>33.134999999999998</v>
+      </c>
+      <c r="Q44">
+        <v>32.481999999999999</v>
+      </c>
+      <c r="R44">
+        <v>31.809000000000001</v>
+      </c>
+      <c r="S44">
+        <v>31.132999999999999</v>
+      </c>
+      <c r="T44">
+        <v>30.471</v>
+      </c>
+      <c r="U44">
+        <v>29.841000000000001</v>
+      </c>
+      <c r="V44">
+        <v>29.234000000000002</v>
+      </c>
+      <c r="W44">
+        <v>28.632999999999999</v>
+      </c>
+      <c r="X44">
+        <v>28.041</v>
+      </c>
+      <c r="Y44">
+        <v>27.46</v>
+      </c>
+      <c r="Z44">
+        <v>26.895</v>
+      </c>
+      <c r="AA44">
+        <v>26.349</v>
+      </c>
+      <c r="AB44">
+        <v>25.841999999999999</v>
+      </c>
+      <c r="AC44">
+        <v>25.379000000000001</v>
+      </c>
+      <c r="AD44">
+        <v>24.940999999999999</v>
+      </c>
+      <c r="AE44">
+        <v>24.506</v>
+      </c>
+      <c r="AF44">
+        <v>24.056000000000001</v>
+      </c>
+      <c r="AG44">
+        <v>23.568999999999999</v>
+      </c>
+      <c r="AH44">
+        <v>23.027000000000001</v>
+      </c>
+      <c r="AI44">
+        <v>22.408000000000001</v>
+      </c>
+      <c r="AJ44">
+        <v>21.574999999999999</v>
+      </c>
+      <c r="AK44">
+        <v>21.05</v>
+      </c>
+      <c r="AL44">
+        <v>20.632999999999999</v>
+      </c>
+      <c r="AM44">
+        <v>20.268000000000001</v>
+      </c>
+      <c r="AN44">
+        <v>19.899000000000001</v>
+      </c>
+      <c r="AO44">
+        <v>19.535</v>
+      </c>
+      <c r="AP44">
+        <v>19.187000000000001</v>
+      </c>
+      <c r="AQ44">
+        <v>18.800999999999998</v>
+      </c>
+      <c r="AR44">
+        <v>18.311</v>
+      </c>
+      <c r="AS44">
+        <v>17.77</v>
+      </c>
+      <c r="AT44">
+        <v>17.302</v>
+      </c>
+      <c r="AU44">
+        <v>16.925000000000001</v>
+      </c>
+      <c r="AV44">
+        <v>16.581</v>
+      </c>
+      <c r="AW44">
+        <v>16.283000000000001</v>
+      </c>
+      <c r="AX44">
+        <v>16.042000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="B45">
+        <v>3.3959999999999999</v>
+      </c>
+      <c r="C45">
+        <v>1.93</v>
+      </c>
+      <c r="D45">
+        <v>9.3190000000000008</v>
+      </c>
+      <c r="E45">
+        <v>12.391999999999999</v>
+      </c>
+      <c r="F45">
+        <v>14.154</v>
+      </c>
+      <c r="G45">
+        <v>15.906000000000001</v>
+      </c>
+      <c r="H45">
+        <v>17.152999999999999</v>
+      </c>
+      <c r="I45">
+        <v>13.397</v>
+      </c>
+      <c r="J45">
+        <v>18.827999999999999</v>
+      </c>
+      <c r="K45">
+        <v>20.684999999999999</v>
+      </c>
+      <c r="L45">
+        <v>19.873000000000001</v>
+      </c>
+      <c r="M45">
+        <v>19.885999999999999</v>
+      </c>
+      <c r="N45">
+        <v>20.763999999999999</v>
+      </c>
+      <c r="O45">
+        <v>21.225000000000001</v>
+      </c>
+      <c r="P45">
+        <v>21.638000000000002</v>
+      </c>
+      <c r="Q45">
+        <v>21.995000000000001</v>
+      </c>
+      <c r="R45">
+        <v>22.286999999999999</v>
+      </c>
+      <c r="S45">
+        <v>22.506</v>
+      </c>
+      <c r="T45">
+        <v>22.643000000000001</v>
+      </c>
+      <c r="U45">
+        <v>22.690999999999999</v>
+      </c>
+      <c r="V45">
+        <v>22.218</v>
+      </c>
+      <c r="W45">
+        <v>21.029</v>
+      </c>
+      <c r="X45">
+        <v>19.47</v>
+      </c>
+      <c r="Y45">
+        <v>17.888000000000002</v>
+      </c>
+      <c r="Z45">
+        <v>16.63</v>
+      </c>
+      <c r="AA45">
+        <v>16.041</v>
+      </c>
+      <c r="AB45">
+        <v>15.926</v>
+      </c>
+      <c r="AC45">
+        <v>15.851000000000001</v>
+      </c>
+      <c r="AD45">
+        <v>15.801</v>
+      </c>
+      <c r="AE45">
+        <v>15.763999999999999</v>
+      </c>
+      <c r="AF45">
+        <v>15.727</v>
+      </c>
+      <c r="AG45">
+        <v>15.675000000000001</v>
+      </c>
+      <c r="AH45">
+        <v>15.596</v>
+      </c>
+      <c r="AI45">
+        <v>15.476000000000001</v>
+      </c>
+      <c r="AJ45">
+        <v>15.1</v>
+      </c>
+      <c r="AK45">
+        <v>14.776999999999999</v>
+      </c>
+      <c r="AL45">
+        <v>14.481999999999999</v>
+      </c>
+      <c r="AM45">
+        <v>14.176</v>
+      </c>
+      <c r="AN45">
+        <v>13.815</v>
+      </c>
+      <c r="AO45">
+        <v>13.278</v>
+      </c>
+      <c r="AP45">
+        <v>12.662000000000001</v>
+      </c>
+      <c r="AQ45">
+        <v>12.252000000000001</v>
+      </c>
+      <c r="AR45">
+        <v>12.086</v>
+      </c>
+      <c r="AS45">
+        <v>11.973000000000001</v>
+      </c>
+      <c r="AT45">
+        <v>11.852</v>
+      </c>
+      <c r="AU45">
+        <v>11.702</v>
+      </c>
+      <c r="AV45">
+        <v>11.544</v>
+      </c>
+      <c r="AW45">
+        <v>11.377000000000001</v>
+      </c>
+      <c r="AX45">
+        <v>11.202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>6.5839999999999996</v>
+      </c>
+      <c r="B46">
+        <v>14.368</v>
+      </c>
+      <c r="C46">
+        <v>19.504000000000001</v>
+      </c>
+      <c r="D46">
+        <v>21.738</v>
+      </c>
+      <c r="E46">
+        <v>22.614999999999998</v>
+      </c>
+      <c r="F46">
+        <v>21.716999999999999</v>
+      </c>
+      <c r="G46">
+        <v>21.170999999999999</v>
+      </c>
+      <c r="H46">
+        <v>19.776</v>
+      </c>
+      <c r="I46">
+        <v>16.832999999999998</v>
+      </c>
+      <c r="J46">
+        <v>17.669</v>
+      </c>
+      <c r="K46">
+        <v>16.405999999999999</v>
+      </c>
+      <c r="L46">
+        <v>15.391999999999999</v>
+      </c>
+      <c r="M46">
+        <v>14.465</v>
+      </c>
+      <c r="N46">
+        <v>13.581</v>
+      </c>
+      <c r="O46">
+        <v>12.813000000000001</v>
+      </c>
+      <c r="P46">
+        <v>12.051</v>
+      </c>
+      <c r="Q46">
+        <v>11.321</v>
+      </c>
+      <c r="R46">
+        <v>10.648</v>
+      </c>
+      <c r="S46">
+        <v>10.058999999999999</v>
+      </c>
+      <c r="T46">
+        <v>9.5779999999999994</v>
+      </c>
+      <c r="U46">
+        <v>9.2319999999999993</v>
+      </c>
+      <c r="V46">
+        <v>9.0009999999999994</v>
+      </c>
+      <c r="W46">
+        <v>8.8290000000000006</v>
+      </c>
+      <c r="X46">
+        <v>8.6880000000000006</v>
+      </c>
+      <c r="Y46">
+        <v>8.5510000000000002</v>
+      </c>
+      <c r="Z46">
+        <v>8.39</v>
+      </c>
+      <c r="AA46">
+        <v>8.1769999999999996</v>
+      </c>
+      <c r="AB46">
+        <v>7.8360000000000003</v>
+      </c>
+      <c r="AC46">
+        <v>7.3479999999999999</v>
+      </c>
+      <c r="AD46">
+        <v>6.77</v>
+      </c>
+      <c r="AE46">
+        <v>6.1609999999999996</v>
+      </c>
+      <c r="AF46">
+        <v>5.58</v>
+      </c>
+      <c r="AG46">
+        <v>5.0830000000000002</v>
+      </c>
+      <c r="AH46">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="AI46">
+        <v>4.5789999999999997</v>
+      </c>
+      <c r="AJ46">
+        <v>4.5590000000000002</v>
+      </c>
+      <c r="AK46">
+        <v>4.4349999999999996</v>
+      </c>
+      <c r="AL46">
+        <v>4.1849999999999996</v>
+      </c>
+      <c r="AM46">
+        <v>3.903</v>
+      </c>
+      <c r="AN46">
+        <v>3.6819999999999999</v>
+      </c>
+      <c r="AO46">
+        <v>3.54</v>
+      </c>
+      <c r="AP46">
+        <v>3.419</v>
+      </c>
+      <c r="AQ46">
+        <v>3.294</v>
+      </c>
+      <c r="AR46">
+        <v>3.15</v>
+      </c>
+      <c r="AS46">
+        <v>3.0009999999999999</v>
+      </c>
+      <c r="AT46">
+        <v>2.8650000000000002</v>
+      </c>
+      <c r="AU46">
+        <v>2.7450000000000001</v>
+      </c>
+      <c r="AV46">
+        <v>2.633</v>
+      </c>
+      <c r="AW46">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="AX46">
+        <v>2.4369999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>20</v>
+      </c>
+      <c r="B47">
+        <v>20</v>
+      </c>
+      <c r="C47">
+        <v>20</v>
+      </c>
+      <c r="D47">
+        <v>20</v>
+      </c>
+      <c r="E47">
+        <v>20</v>
+      </c>
+      <c r="F47">
+        <v>20</v>
+      </c>
+      <c r="G47">
+        <v>20</v>
+      </c>
+      <c r="H47">
+        <v>20</v>
+      </c>
+      <c r="I47">
+        <v>20</v>
+      </c>
+      <c r="J47">
+        <v>20</v>
+      </c>
+      <c r="K47">
+        <v>20</v>
+      </c>
+      <c r="L47">
+        <v>20</v>
+      </c>
+      <c r="M47">
+        <v>20</v>
+      </c>
+      <c r="N47">
+        <v>20</v>
+      </c>
+      <c r="O47">
+        <v>20</v>
+      </c>
+      <c r="P47">
+        <v>20</v>
+      </c>
+      <c r="Q47">
+        <v>20</v>
+      </c>
+      <c r="R47">
+        <v>20</v>
+      </c>
+      <c r="S47">
+        <v>20</v>
+      </c>
+      <c r="T47">
+        <v>20</v>
+      </c>
+      <c r="U47">
+        <v>20</v>
+      </c>
+      <c r="V47">
+        <v>20</v>
+      </c>
+      <c r="W47">
+        <v>20</v>
+      </c>
+      <c r="X47">
+        <v>20</v>
+      </c>
+      <c r="Y47">
+        <v>20</v>
+      </c>
+      <c r="Z47">
+        <v>20</v>
+      </c>
+      <c r="AA47">
+        <v>20</v>
+      </c>
+      <c r="AB47">
+        <v>20</v>
+      </c>
+      <c r="AC47">
+        <v>20</v>
+      </c>
+      <c r="AD47">
+        <v>20</v>
+      </c>
+      <c r="AE47">
+        <v>20</v>
+      </c>
+      <c r="AF47">
+        <v>20</v>
+      </c>
+      <c r="AG47">
+        <v>20</v>
+      </c>
+      <c r="AH47">
+        <v>20</v>
+      </c>
+      <c r="AI47">
+        <v>20</v>
+      </c>
+      <c r="AJ47">
+        <v>20</v>
+      </c>
+      <c r="AK47">
+        <v>20</v>
+      </c>
+      <c r="AL47">
+        <v>20</v>
+      </c>
+      <c r="AM47">
+        <v>20</v>
+      </c>
+      <c r="AN47">
+        <v>20</v>
+      </c>
+      <c r="AO47">
+        <v>20</v>
+      </c>
+      <c r="AP47">
+        <v>20</v>
+      </c>
+      <c r="AQ47">
+        <v>20</v>
+      </c>
+      <c r="AR47">
+        <v>20</v>
+      </c>
+      <c r="AS47">
+        <v>20</v>
+      </c>
+      <c r="AT47">
+        <v>20</v>
+      </c>
+      <c r="AU47">
+        <v>20</v>
+      </c>
+      <c r="AV47">
+        <v>20</v>
+      </c>
+      <c r="AW47">
+        <v>20</v>
+      </c>
+      <c r="AX47">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B48">
+        <v>1.2</v>
+      </c>
+      <c r="C48">
+        <v>1.3</v>
+      </c>
+      <c r="D48">
+        <v>1.4</v>
+      </c>
+      <c r="E48">
+        <v>1.5</v>
+      </c>
+      <c r="F48">
+        <v>1.6</v>
+      </c>
+      <c r="G48">
+        <v>1.7</v>
+      </c>
+      <c r="H48">
+        <v>1.8</v>
+      </c>
+      <c r="I48">
+        <v>1.9</v>
+      </c>
+      <c r="J48">
+        <v>2</v>
+      </c>
+      <c r="K48">
+        <v>2.1</v>
+      </c>
+      <c r="L48">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M48">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N48">
+        <v>2.4</v>
+      </c>
+      <c r="O48">
+        <v>2.5</v>
+      </c>
+      <c r="P48">
+        <v>2.6</v>
+      </c>
+      <c r="Q48">
+        <v>2.7</v>
+      </c>
+      <c r="R48">
+        <v>2.8</v>
+      </c>
+      <c r="S48">
+        <v>2.9</v>
+      </c>
+      <c r="T48">
+        <v>3</v>
+      </c>
+      <c r="U48">
+        <v>3.1</v>
+      </c>
+      <c r="V48">
+        <v>3.2</v>
+      </c>
+      <c r="W48">
+        <v>3.3</v>
+      </c>
+      <c r="X48">
+        <v>3.4</v>
+      </c>
+      <c r="Y48">
+        <v>3.5</v>
+      </c>
+      <c r="Z48">
+        <v>3.6</v>
+      </c>
+      <c r="AA48">
+        <v>3.7</v>
+      </c>
+      <c r="AB48">
+        <v>3.8</v>
+      </c>
+      <c r="AC48">
+        <v>3.9</v>
+      </c>
+      <c r="AD48">
+        <v>4</v>
+      </c>
+      <c r="AE48">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AF48">
+        <v>4.2</v>
+      </c>
+      <c r="AG48">
+        <v>4.3</v>
+      </c>
+      <c r="AH48">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AI48">
+        <v>4.5</v>
+      </c>
+      <c r="AJ48">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AK48">
+        <v>4.7</v>
+      </c>
+      <c r="AL48">
+        <v>4.8</v>
+      </c>
+      <c r="AM48">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="AN48">
+        <v>5</v>
+      </c>
+      <c r="AO48">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AP48">
+        <v>5.2</v>
+      </c>
+      <c r="AQ48">
+        <v>5.3</v>
+      </c>
+      <c r="AR48">
+        <v>5.4</v>
+      </c>
+      <c r="AS48">
+        <v>5.5</v>
+      </c>
+      <c r="AT48">
+        <v>5.6</v>
+      </c>
+      <c r="AU48">
+        <v>5.7</v>
+      </c>
+      <c r="AV48">
+        <v>5.8</v>
+      </c>
+      <c r="AW48">
+        <v>5.9</v>
+      </c>
+      <c r="AX48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>7.1959999999999997</v>
+      </c>
+      <c r="B49">
+        <v>15.981999999999999</v>
+      </c>
+      <c r="C49">
+        <v>26.283999999999999</v>
+      </c>
+      <c r="D49">
+        <v>32.046999999999997</v>
+      </c>
+      <c r="E49">
+        <v>37.659999999999997</v>
+      </c>
+      <c r="F49">
+        <v>34.978999999999999</v>
+      </c>
+      <c r="G49">
+        <v>36.915999999999997</v>
+      </c>
+      <c r="H49">
+        <v>37.012</v>
+      </c>
+      <c r="I49">
+        <v>36.354999999999997</v>
+      </c>
+      <c r="J49">
+        <v>32.981000000000002</v>
+      </c>
+      <c r="K49">
+        <v>35.247999999999998</v>
+      </c>
+      <c r="L49">
+        <v>35.186999999999998</v>
+      </c>
+      <c r="M49">
+        <v>34.131</v>
+      </c>
+      <c r="N49">
+        <v>33.435000000000002</v>
+      </c>
+      <c r="O49">
+        <v>32.741</v>
+      </c>
+      <c r="P49">
+        <v>32.042999999999999</v>
+      </c>
+      <c r="Q49">
+        <v>31.344999999999999</v>
+      </c>
+      <c r="R49">
+        <v>30.654</v>
+      </c>
+      <c r="S49">
+        <v>29.975000000000001</v>
+      </c>
+      <c r="T49">
+        <v>29.312999999999999</v>
+      </c>
+      <c r="U49">
+        <v>28.673999999999999</v>
+      </c>
+      <c r="V49">
+        <v>28.053999999999998</v>
+      </c>
+      <c r="W49">
+        <v>27.446000000000002</v>
+      </c>
+      <c r="X49">
+        <v>26.853000000000002</v>
+      </c>
+      <c r="Y49">
+        <v>26.277000000000001</v>
+      </c>
+      <c r="Z49">
+        <v>25.72</v>
+      </c>
+      <c r="AA49">
+        <v>25.184000000000001</v>
+      </c>
+      <c r="AB49">
+        <v>24.696999999999999</v>
+      </c>
+      <c r="AC49">
+        <v>24.265999999999998</v>
+      </c>
+      <c r="AD49">
+        <v>23.866</v>
+      </c>
+      <c r="AE49">
+        <v>23.47</v>
+      </c>
+      <c r="AF49">
+        <v>23.050999999999998</v>
+      </c>
+      <c r="AG49">
+        <v>22.584</v>
+      </c>
+      <c r="AH49">
+        <v>22.042000000000002</v>
+      </c>
+      <c r="AI49">
+        <v>21.398</v>
+      </c>
+      <c r="AJ49">
+        <v>20.413</v>
+      </c>
+      <c r="AK49">
+        <v>19.763999999999999</v>
+      </c>
+      <c r="AL49">
+        <v>19.218</v>
+      </c>
+      <c r="AM49">
+        <v>18.783000000000001</v>
+      </c>
+      <c r="AN49">
+        <v>18.466000000000001</v>
+      </c>
+      <c r="AO49">
+        <v>18.279</v>
+      </c>
+      <c r="AP49">
+        <v>18.143000000000001</v>
+      </c>
+      <c r="AQ49">
+        <v>17.931000000000001</v>
+      </c>
+      <c r="AR49">
+        <v>17.300999999999998</v>
+      </c>
+      <c r="AS49">
+        <v>16.332999999999998</v>
+      </c>
+      <c r="AT49">
+        <v>15.535</v>
+      </c>
+      <c r="AU49">
+        <v>15.010999999999999</v>
+      </c>
+      <c r="AV49">
+        <v>14.547000000000001</v>
+      </c>
+      <c r="AW49">
+        <v>14.176</v>
+      </c>
+      <c r="AX49">
+        <v>13.928000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="B50">
+        <v>1.143</v>
+      </c>
+      <c r="C50">
+        <v>6.0449999999999999</v>
+      </c>
+      <c r="D50">
+        <v>8.7490000000000006</v>
+      </c>
+      <c r="E50">
+        <v>13.711</v>
+      </c>
+      <c r="F50">
+        <v>11.441000000000001</v>
+      </c>
+      <c r="G50">
+        <v>15.009</v>
+      </c>
+      <c r="H50">
+        <v>16.712</v>
+      </c>
+      <c r="I50">
+        <v>17.091999999999999</v>
+      </c>
+      <c r="J50">
+        <v>14.356</v>
+      </c>
+      <c r="K50">
+        <v>19.288</v>
+      </c>
+      <c r="L50">
+        <v>18.48</v>
+      </c>
+      <c r="M50">
+        <v>18.963000000000001</v>
+      </c>
+      <c r="N50">
+        <v>19.484000000000002</v>
+      </c>
+      <c r="O50">
+        <v>19.459</v>
+      </c>
+      <c r="P50">
+        <v>19.388999999999999</v>
+      </c>
+      <c r="Q50">
+        <v>19.282</v>
+      </c>
+      <c r="R50">
+        <v>19.146000000000001</v>
+      </c>
+      <c r="S50">
+        <v>18.989999999999998</v>
+      </c>
+      <c r="T50">
+        <v>18.821999999999999</v>
+      </c>
+      <c r="U50">
+        <v>18.649000000000001</v>
+      </c>
+      <c r="V50">
+        <v>18.440999999999999</v>
+      </c>
+      <c r="W50">
+        <v>18.173999999999999</v>
+      </c>
+      <c r="X50">
+        <v>17.864999999999998</v>
+      </c>
+      <c r="Y50">
+        <v>17.533000000000001</v>
+      </c>
+      <c r="Z50">
+        <v>17.196999999999999</v>
+      </c>
+      <c r="AA50">
+        <v>16.875</v>
+      </c>
+      <c r="AB50">
+        <v>16.553000000000001</v>
+      </c>
+      <c r="AC50">
+        <v>16.21</v>
+      </c>
+      <c r="AD50">
+        <v>15.856999999999999</v>
+      </c>
+      <c r="AE50">
+        <v>15.503</v>
+      </c>
+      <c r="AF50">
+        <v>15.157999999999999</v>
+      </c>
+      <c r="AG50">
+        <v>14.831</v>
+      </c>
+      <c r="AH50">
+        <v>14.532</v>
+      </c>
+      <c r="AI50">
+        <v>14.27</v>
+      </c>
+      <c r="AJ50">
+        <v>14.061999999999999</v>
+      </c>
+      <c r="AK50">
+        <v>14.667</v>
+      </c>
+      <c r="AL50">
+        <v>15.999000000000001</v>
+      </c>
+      <c r="AM50">
+        <v>17.331</v>
+      </c>
+      <c r="AN50">
+        <v>17.936</v>
+      </c>
+      <c r="AO50">
+        <v>16.225999999999999</v>
+      </c>
+      <c r="AP50">
+        <v>13.052</v>
+      </c>
+      <c r="AQ50">
+        <v>11.342000000000001</v>
+      </c>
+      <c r="AR50">
+        <v>12.526</v>
+      </c>
+      <c r="AS50">
+        <v>14.725</v>
+      </c>
+      <c r="AT50">
+        <v>15.909000000000001</v>
+      </c>
+      <c r="AU50">
+        <v>15.349</v>
+      </c>
+      <c r="AV50">
+        <v>13.686</v>
+      </c>
+      <c r="AW50">
+        <v>10.945</v>
+      </c>
+      <c r="AX50">
+        <v>7.1529999999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>6.6059999999999999</v>
+      </c>
+      <c r="B51">
+        <v>15.243</v>
+      </c>
+      <c r="C51">
+        <v>20.149000000000001</v>
+      </c>
+      <c r="D51">
+        <v>22.49</v>
+      </c>
+      <c r="E51">
+        <v>23.887</v>
+      </c>
+      <c r="F51">
+        <v>22.695</v>
+      </c>
+      <c r="G51">
+        <v>21.614000000000001</v>
+      </c>
+      <c r="H51">
+        <v>20.48</v>
+      </c>
+      <c r="I51">
+        <v>19.303999999999998</v>
+      </c>
+      <c r="J51">
+        <v>17.163</v>
+      </c>
+      <c r="K51">
+        <v>17.027999999999999</v>
+      </c>
+      <c r="L51">
+        <v>15.87</v>
+      </c>
+      <c r="M51">
+        <v>14.972</v>
+      </c>
+      <c r="N51">
+        <v>14.180999999999999</v>
+      </c>
+      <c r="O51">
+        <v>13.427</v>
+      </c>
+      <c r="P51">
+        <v>12.670999999999999</v>
+      </c>
+      <c r="Q51">
+        <v>11.927</v>
+      </c>
+      <c r="R51">
+        <v>11.211</v>
+      </c>
+      <c r="S51">
+        <v>10.536</v>
+      </c>
+      <c r="T51">
+        <v>9.9160000000000004</v>
+      </c>
+      <c r="U51">
+        <v>9.3670000000000009</v>
+      </c>
+      <c r="V51">
+        <v>8.8759999999999994</v>
+      </c>
+      <c r="W51">
+        <v>8.423</v>
+      </c>
+      <c r="X51">
+        <v>8.0030000000000001</v>
+      </c>
+      <c r="Y51">
+        <v>7.6130000000000004</v>
+      </c>
+      <c r="Z51">
+        <v>7.25</v>
+      </c>
+      <c r="AA51">
+        <v>6.91</v>
+      </c>
+      <c r="AB51">
+        <v>6.5860000000000003</v>
+      </c>
+      <c r="AC51">
+        <v>6.274</v>
+      </c>
+      <c r="AD51">
+        <v>5.976</v>
+      </c>
+      <c r="AE51">
+        <v>5.6920000000000002</v>
+      </c>
+      <c r="AF51">
+        <v>5.4249999999999998</v>
+      </c>
+      <c r="AG51">
+        <v>5.1769999999999996</v>
+      </c>
+      <c r="AH51">
+        <v>4.9489999999999998</v>
+      </c>
+      <c r="AI51">
+        <v>4.7439999999999998</v>
+      </c>
+      <c r="AJ51">
+        <v>4.577</v>
+      </c>
+      <c r="AK51">
+        <v>4.42</v>
+      </c>
+      <c r="AL51">
+        <v>4.2679999999999998</v>
+      </c>
+      <c r="AM51">
+        <v>4.1130000000000004</v>
+      </c>
+      <c r="AN51">
+        <v>3.9470000000000001</v>
+      </c>
+      <c r="AO51">
+        <v>3.7519999999999998</v>
+      </c>
+      <c r="AP51">
+        <v>3.5430000000000001</v>
+      </c>
+      <c r="AQ51">
+        <v>3.3639999999999999</v>
+      </c>
+      <c r="AR51">
+        <v>3.2029999999999998</v>
+      </c>
+      <c r="AS51">
+        <v>3.06</v>
+      </c>
+      <c r="AT51">
+        <v>2.9980000000000002</v>
+      </c>
+      <c r="AU51">
+        <v>3.125</v>
+      </c>
+      <c r="AV51">
+        <v>3.4769999999999999</v>
+      </c>
+      <c r="AW51">
+        <v>4.0119999999999996</v>
+      </c>
+      <c r="AX51">
+        <v>4.6890000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fehler in Excel korrigiert
</commit_message>
<xml_diff>
--- a/magnet.xlsx
+++ b/magnet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git-Repositories\Streamlit_Magnetgetriebe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C21F9A-34ED-4233-A6A7-2BC259943DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0B29BE-CC0D-4318-89CC-DD716086C7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F30568EE-B3B4-42DF-9CF1-B5E536E04381}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F30568EE-B3B4-42DF-9CF1-B5E536E04381}"/>
   </bookViews>
   <sheets>
     <sheet name="test2" sheetId="1" r:id="rId1"/>
@@ -893,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB0DFE6-30A2-4A15-91CE-18FDCD3EAF8D}">
   <dimension ref="A1:AX51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE28" workbookViewId="0">
-      <selection activeCell="AY42" sqref="AY42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5765,458 +5765,458 @@
     </row>
     <row r="33" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>1.1428571428571428</v>
+        <v>8</v>
       </c>
       <c r="B33">
-        <v>1.2857142857142856</v>
+        <v>9</v>
       </c>
       <c r="C33">
-        <v>1.4285714285714286</v>
+        <v>10</v>
       </c>
       <c r="D33">
-        <v>1.5714285714285714</v>
+        <v>11</v>
       </c>
       <c r="E33">
-        <v>1.7142857142857144</v>
+        <v>12</v>
       </c>
       <c r="F33">
-        <v>1.8571428571428572</v>
+        <v>13</v>
       </c>
       <c r="G33">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H33">
-        <v>2.1428571428571428</v>
+        <v>15</v>
       </c>
       <c r="I33">
-        <v>2.2857142857142856</v>
+        <v>16</v>
       </c>
       <c r="J33">
-        <v>2.4285714285714288</v>
+        <v>17</v>
       </c>
       <c r="K33">
-        <v>2.5714285714285712</v>
+        <v>18</v>
       </c>
       <c r="L33">
-        <v>2.7142857142857144</v>
+        <v>19</v>
       </c>
       <c r="M33">
-        <v>2.8571428571428572</v>
+        <v>20</v>
       </c>
       <c r="N33">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="O33">
-        <v>3.1428571428571428</v>
+        <v>22</v>
       </c>
       <c r="P33">
-        <v>3.2857142857142856</v>
+        <v>23</v>
       </c>
       <c r="Q33">
-        <v>3.4285714285714284</v>
+        <v>24</v>
       </c>
       <c r="R33">
-        <v>3.5714285714285716</v>
+        <v>25</v>
       </c>
       <c r="S33">
-        <v>3.7142857142857144</v>
+        <v>26</v>
       </c>
       <c r="T33">
-        <v>3.8571428571428572</v>
+        <v>27</v>
       </c>
       <c r="U33">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="V33">
-        <v>4.1428571428571423</v>
+        <v>29</v>
       </c>
       <c r="W33">
-        <v>4.2857142857142856</v>
+        <v>30</v>
       </c>
       <c r="X33">
-        <v>4.4285714285714288</v>
+        <v>31</v>
       </c>
       <c r="Y33">
-        <v>4.5714285714285712</v>
+        <v>32</v>
       </c>
       <c r="Z33">
-        <v>4.7142857142857144</v>
+        <v>33</v>
       </c>
       <c r="AA33">
-        <v>4.8571428571428577</v>
+        <v>34</v>
       </c>
       <c r="AB33">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="AC33">
-        <v>5.1428571428571432</v>
+        <v>36</v>
       </c>
       <c r="AD33">
-        <v>5.2857142857142856</v>
+        <v>37</v>
       </c>
       <c r="AE33">
-        <v>5.4285714285714288</v>
+        <v>38</v>
       </c>
       <c r="AF33">
-        <v>5.5714285714285712</v>
+        <v>39</v>
       </c>
       <c r="AG33">
-        <v>5.7142857142857144</v>
+        <v>40</v>
       </c>
       <c r="AH33">
-        <v>5.8571428571428568</v>
+        <v>41</v>
       </c>
       <c r="AI33">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="AJ33">
-        <v>6.1428571428571432</v>
+        <v>43</v>
       </c>
       <c r="AK33">
-        <v>6.2857142857142856</v>
+        <v>44</v>
       </c>
       <c r="AL33">
-        <v>6.4285714285714288</v>
+        <v>45</v>
       </c>
       <c r="AM33">
-        <v>6.5714285714285712</v>
+        <v>46</v>
       </c>
       <c r="AN33">
-        <v>6.7142857142857144</v>
+        <v>47</v>
       </c>
       <c r="AO33">
-        <v>6.8571428571428568</v>
+        <v>48</v>
       </c>
       <c r="AP33">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="AQ33">
-        <v>7.1428571428571432</v>
+        <v>50</v>
       </c>
       <c r="AR33">
-        <v>7.2857142857142856</v>
+        <v>51</v>
       </c>
       <c r="AS33">
-        <v>7.4285714285714288</v>
+        <v>52</v>
       </c>
       <c r="AT33">
-        <v>7.5714285714285712</v>
+        <v>53</v>
       </c>
       <c r="AU33">
-        <v>7.7142857142857144</v>
+        <v>54</v>
       </c>
       <c r="AV33">
-        <v>7.8571428571428568</v>
+        <v>55</v>
       </c>
       <c r="AW33">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="AX33">
-        <v>8.1428571428571423</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>6.8550000000000004</v>
+        <v>1.1428571428571428</v>
       </c>
       <c r="B34">
-        <v>17.55</v>
+        <v>1.2857142857142856</v>
       </c>
       <c r="C34">
-        <v>24.427</v>
+        <v>1.4285714285714286</v>
       </c>
       <c r="D34">
-        <v>31.541</v>
+        <v>1.5714285714285714</v>
       </c>
       <c r="E34">
-        <v>34.264000000000003</v>
+        <v>1.7142857142857144</v>
       </c>
       <c r="F34">
-        <v>36.984999999999999</v>
+        <v>1.8571428571428572</v>
       </c>
       <c r="G34">
-        <v>25.550999999999998</v>
+        <v>2</v>
       </c>
       <c r="H34">
-        <v>38.777999999999999</v>
+        <v>2.1428571428571428</v>
       </c>
       <c r="I34">
-        <v>38.061</v>
+        <v>2.2857142857142856</v>
       </c>
       <c r="J34">
-        <v>37.593000000000004</v>
+        <v>2.4285714285714288</v>
       </c>
       <c r="K34">
-        <v>37.298999999999999</v>
+        <v>2.5714285714285712</v>
       </c>
       <c r="L34">
-        <v>37.563000000000002</v>
+        <v>2.7142857142857144</v>
       </c>
       <c r="M34">
-        <v>36.406999999999996</v>
+        <v>2.8571428571428572</v>
       </c>
       <c r="N34">
-        <v>37.578000000000003</v>
+        <v>3</v>
       </c>
       <c r="O34">
-        <v>37.390999999999998</v>
+        <v>3.1428571428571428</v>
       </c>
       <c r="P34">
-        <v>36.863</v>
+        <v>3.2857142857142856</v>
       </c>
       <c r="Q34">
-        <v>36.045000000000002</v>
+        <v>3.4285714285714284</v>
       </c>
       <c r="R34">
-        <v>34.987000000000002</v>
+        <v>3.5714285714285716</v>
       </c>
       <c r="S34">
-        <v>33.74</v>
+        <v>3.7142857142857144</v>
       </c>
       <c r="T34">
-        <v>32.351999999999997</v>
+        <v>3.8571428571428572</v>
       </c>
       <c r="U34">
-        <v>29.940999999999999</v>
+        <v>4</v>
       </c>
       <c r="V34">
-        <v>31.099</v>
+        <v>4.1428571428571423</v>
       </c>
       <c r="W34">
-        <v>28.72</v>
+        <v>4.2857142857142856</v>
       </c>
       <c r="X34">
-        <v>24.3</v>
+        <v>4.4285714285714288</v>
       </c>
       <c r="Y34">
-        <v>21.920999999999999</v>
+        <v>4.5714285714285712</v>
       </c>
       <c r="Z34">
-        <v>25.283999999999999</v>
+        <v>4.7142857142857144</v>
       </c>
       <c r="AA34">
-        <v>28.646999999999998</v>
+        <v>4.8571428571428577</v>
       </c>
       <c r="AB34">
-        <v>28.439</v>
+        <v>5</v>
       </c>
       <c r="AC34">
-        <v>27.9</v>
+        <v>5.1428571428571432</v>
       </c>
       <c r="AD34">
-        <v>27.158999999999999</v>
+        <v>5.2857142857142856</v>
       </c>
       <c r="AE34">
-        <v>26.344999999999999</v>
+        <v>5.4285714285714288</v>
       </c>
       <c r="AF34">
-        <v>25.042999999999999</v>
+        <v>5.5714285714285712</v>
       </c>
       <c r="AG34">
-        <v>23.23</v>
+        <v>5.7142857142857144</v>
       </c>
       <c r="AH34">
-        <v>21.619</v>
+        <v>5.8571428571428568</v>
       </c>
       <c r="AI34">
-        <v>20.922999999999998</v>
+        <v>6</v>
       </c>
       <c r="AJ34">
-        <v>23.452000000000002</v>
+        <v>6.1428571428571432</v>
       </c>
       <c r="AK34">
-        <v>23.355</v>
+        <v>6.2857142857142856</v>
       </c>
       <c r="AL34">
-        <v>23.088999999999999</v>
+        <v>6.4285714285714288</v>
       </c>
       <c r="AM34">
-        <v>22.693999999999999</v>
+        <v>6.5714285714285712</v>
       </c>
       <c r="AN34">
-        <v>22.209</v>
+        <v>6.7142857142857144</v>
       </c>
       <c r="AO34">
-        <v>21.672999999999998</v>
+        <v>6.8571428571428568</v>
       </c>
       <c r="AP34">
-        <v>21.125</v>
+        <v>7</v>
       </c>
       <c r="AQ34">
-        <v>20.605</v>
+        <v>7.1428571428571432</v>
       </c>
       <c r="AR34">
-        <v>20.027999999999999</v>
+        <v>7.2857142857142856</v>
       </c>
       <c r="AS34">
-        <v>19.36</v>
+        <v>7.4285714285714288</v>
       </c>
       <c r="AT34">
-        <v>18.713999999999999</v>
+        <v>7.5714285714285712</v>
       </c>
       <c r="AU34">
-        <v>18.202999999999999</v>
+        <v>7.7142857142857144</v>
       </c>
       <c r="AV34">
-        <v>17.821000000000002</v>
+        <v>7.8571428571428568</v>
       </c>
       <c r="AW34">
-        <v>17.5</v>
+        <v>8</v>
       </c>
       <c r="AX34">
-        <v>17.260999999999999</v>
+        <v>8.1428571428571423</v>
       </c>
     </row>
     <row r="35" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>0.69299999999999995</v>
+        <v>6.8550000000000004</v>
       </c>
       <c r="B35">
-        <v>4.0229999999999997</v>
+        <v>17.55</v>
       </c>
       <c r="C35">
-        <v>7.1710000000000003</v>
+        <v>24.427</v>
       </c>
       <c r="D35">
-        <v>11.113</v>
+        <v>31.541</v>
       </c>
       <c r="E35">
-        <v>14.239000000000001</v>
+        <v>34.264000000000003</v>
       </c>
       <c r="F35">
-        <v>16.637</v>
+        <v>36.984999999999999</v>
       </c>
       <c r="G35">
-        <v>10.920999999999999</v>
+        <v>25.550999999999998</v>
       </c>
       <c r="H35">
-        <v>20.013000000000002</v>
+        <v>38.777999999999999</v>
       </c>
       <c r="I35">
-        <v>22.559000000000001</v>
+        <v>38.061</v>
       </c>
       <c r="J35">
-        <v>23.472999999999999</v>
+        <v>37.593000000000004</v>
       </c>
       <c r="K35">
-        <v>23.065999999999999</v>
+        <v>37.298999999999999</v>
       </c>
       <c r="L35">
-        <v>24.228999999999999</v>
+        <v>37.563000000000002</v>
       </c>
       <c r="M35">
-        <v>24.739000000000001</v>
+        <v>36.406999999999996</v>
       </c>
       <c r="N35">
-        <v>25.795999999999999</v>
+        <v>37.578000000000003</v>
       </c>
       <c r="O35">
-        <v>25.751000000000001</v>
+        <v>37.390999999999998</v>
       </c>
       <c r="P35">
-        <v>25.606000000000002</v>
+        <v>36.863</v>
       </c>
       <c r="Q35">
-        <v>25.347000000000001</v>
+        <v>36.045000000000002</v>
       </c>
       <c r="R35">
-        <v>24.957000000000001</v>
+        <v>34.987000000000002</v>
       </c>
       <c r="S35">
-        <v>24.422999999999998</v>
+        <v>33.74</v>
       </c>
       <c r="T35">
-        <v>23.728999999999999</v>
+        <v>32.351999999999997</v>
       </c>
       <c r="U35">
-        <v>20.245000000000001</v>
+        <v>29.940999999999999</v>
       </c>
       <c r="V35">
-        <v>22.49</v>
+        <v>31.099</v>
       </c>
       <c r="W35">
-        <v>22.405999999999999</v>
+        <v>28.72</v>
       </c>
       <c r="X35">
-        <v>22.195</v>
+        <v>24.3</v>
       </c>
       <c r="Y35">
         <v>21.920999999999999</v>
       </c>
       <c r="Z35">
-        <v>21.443999999999999</v>
+        <v>25.283999999999999</v>
       </c>
       <c r="AA35">
-        <v>20.9</v>
+        <v>28.646999999999998</v>
       </c>
       <c r="AB35">
-        <v>20.503</v>
+        <v>28.439</v>
       </c>
       <c r="AC35">
-        <v>20.145</v>
+        <v>27.9</v>
       </c>
       <c r="AD35">
-        <v>19.824000000000002</v>
+        <v>27.158999999999999</v>
       </c>
       <c r="AE35">
-        <v>19.533999999999999</v>
+        <v>26.344999999999999</v>
       </c>
       <c r="AF35">
-        <v>19.236000000000001</v>
+        <v>25.042999999999999</v>
       </c>
       <c r="AG35">
-        <v>18.937000000000001</v>
+        <v>23.23</v>
       </c>
       <c r="AH35">
-        <v>18.706</v>
+        <v>21.619</v>
       </c>
       <c r="AI35">
-        <v>18.614000000000001</v>
+        <v>20.922999999999998</v>
       </c>
       <c r="AJ35">
-        <v>22.16</v>
+        <v>23.452000000000002</v>
       </c>
       <c r="AK35">
-        <v>21.757000000000001</v>
+        <v>23.355</v>
       </c>
       <c r="AL35">
-        <v>20.719000000000001</v>
+        <v>23.088999999999999</v>
       </c>
       <c r="AM35">
-        <v>19.297999999999998</v>
+        <v>22.693999999999999</v>
       </c>
       <c r="AN35">
-        <v>17.751000000000001</v>
+        <v>22.209</v>
       </c>
       <c r="AO35">
-        <v>16.329999999999998</v>
+        <v>21.672999999999998</v>
       </c>
       <c r="AP35">
-        <v>15.292</v>
+        <v>21.125</v>
       </c>
       <c r="AQ35">
-        <v>14.888999999999999</v>
+        <v>20.605</v>
       </c>
       <c r="AR35">
-        <v>15.613</v>
+        <v>20.027999999999999</v>
       </c>
       <c r="AS35">
-        <v>17.207000000000001</v>
+        <v>19.36</v>
       </c>
       <c r="AT35">
-        <v>18.800999999999998</v>
+        <v>18.713999999999999</v>
       </c>
       <c r="AU35">
-        <v>19.524999999999999</v>
+        <v>18.202999999999999</v>
       </c>
       <c r="AV35">
-        <v>19.446999999999999</v>
+        <v>17.821000000000002</v>
       </c>
       <c r="AW35">
-        <v>19.097000000000001</v>
+        <v>17.5</v>
       </c>
       <c r="AX35">
-        <v>18.298999999999999</v>
+        <v>17.260999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:50" x14ac:dyDescent="0.25">
@@ -6525,458 +6525,458 @@
     </row>
     <row r="38" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>1.125</v>
+        <v>9</v>
       </c>
       <c r="B38">
-        <v>1.25</v>
+        <v>10</v>
       </c>
       <c r="C38">
-        <v>1.375</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>1.5</v>
+        <v>12</v>
       </c>
       <c r="E38">
-        <v>1.625</v>
+        <v>13</v>
       </c>
       <c r="F38">
-        <v>1.75</v>
+        <v>14</v>
       </c>
       <c r="G38">
-        <v>1.875</v>
+        <v>15</v>
       </c>
       <c r="H38">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="I38">
-        <v>2.125</v>
+        <v>17</v>
       </c>
       <c r="J38">
-        <v>2.25</v>
+        <v>18</v>
       </c>
       <c r="K38">
-        <v>2.375</v>
+        <v>19</v>
       </c>
       <c r="L38">
-        <v>2.5</v>
+        <v>20</v>
       </c>
       <c r="M38">
-        <v>2.625</v>
+        <v>21</v>
       </c>
       <c r="N38">
-        <v>2.75</v>
+        <v>22</v>
       </c>
       <c r="O38">
-        <v>2.875</v>
+        <v>23</v>
       </c>
       <c r="P38">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="Q38">
-        <v>3.125</v>
+        <v>25</v>
       </c>
       <c r="R38">
-        <v>3.25</v>
+        <v>26</v>
       </c>
       <c r="S38">
-        <v>3.375</v>
+        <v>27</v>
       </c>
       <c r="T38">
-        <v>3.5</v>
+        <v>28</v>
       </c>
       <c r="U38">
-        <v>3.625</v>
+        <v>29</v>
       </c>
       <c r="V38">
-        <v>3.75</v>
+        <v>30</v>
       </c>
       <c r="W38">
-        <v>3.875</v>
+        <v>31</v>
       </c>
       <c r="X38">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="Y38">
-        <v>4.125</v>
+        <v>33</v>
       </c>
       <c r="Z38">
-        <v>4.25</v>
+        <v>34</v>
       </c>
       <c r="AA38">
-        <v>4.375</v>
+        <v>35</v>
       </c>
       <c r="AB38">
-        <v>4.5</v>
+        <v>36</v>
       </c>
       <c r="AC38">
-        <v>4.625</v>
+        <v>37</v>
       </c>
       <c r="AD38">
-        <v>4.75</v>
+        <v>38</v>
       </c>
       <c r="AE38">
-        <v>4.875</v>
+        <v>39</v>
       </c>
       <c r="AF38">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="AG38">
-        <v>5.125</v>
+        <v>41</v>
       </c>
       <c r="AH38">
-        <v>5.25</v>
+        <v>42</v>
       </c>
       <c r="AI38">
-        <v>5.375</v>
+        <v>43</v>
       </c>
       <c r="AJ38">
-        <v>5.5</v>
+        <v>44</v>
       </c>
       <c r="AK38">
-        <v>5.625</v>
+        <v>45</v>
       </c>
       <c r="AL38">
-        <v>5.75</v>
+        <v>46</v>
       </c>
       <c r="AM38">
-        <v>5.875</v>
+        <v>47</v>
       </c>
       <c r="AN38">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="AO38">
-        <v>6.125</v>
+        <v>49</v>
       </c>
       <c r="AP38">
-        <v>6.25</v>
+        <v>50</v>
       </c>
       <c r="AQ38">
-        <v>6.375</v>
+        <v>51</v>
       </c>
       <c r="AR38">
-        <v>6.5</v>
+        <v>52</v>
       </c>
       <c r="AS38">
-        <v>6.625</v>
+        <v>53</v>
       </c>
       <c r="AT38">
-        <v>6.75</v>
+        <v>54</v>
       </c>
       <c r="AU38">
-        <v>6.875</v>
+        <v>55</v>
       </c>
       <c r="AV38">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="AW38">
-        <v>7.125</v>
+        <v>57</v>
       </c>
       <c r="AX38">
-        <v>7.25</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>6.8819999999999997</v>
+        <v>1.125</v>
       </c>
       <c r="B39">
-        <v>18.625</v>
+        <v>1.25</v>
       </c>
       <c r="C39">
-        <v>26.263999999999999</v>
+        <v>1.375</v>
       </c>
       <c r="D39">
-        <v>34.796999999999997</v>
+        <v>1.5</v>
       </c>
       <c r="E39">
-        <v>35.384</v>
+        <v>1.625</v>
       </c>
       <c r="F39">
-        <v>36.887999999999998</v>
+        <v>1.75</v>
       </c>
       <c r="G39">
-        <v>37.512</v>
+        <v>1.875</v>
       </c>
       <c r="H39">
-        <v>28.463000000000001</v>
+        <v>2</v>
       </c>
       <c r="I39">
-        <v>38.103999999999999</v>
+        <v>2.125</v>
       </c>
       <c r="J39">
-        <v>37.331000000000003</v>
+        <v>2.25</v>
       </c>
       <c r="K39">
-        <v>36.798999999999999</v>
+        <v>2.375</v>
       </c>
       <c r="L39">
-        <v>37.634</v>
+        <v>2.5</v>
       </c>
       <c r="M39">
-        <v>36.225999999999999</v>
+        <v>2.625</v>
       </c>
       <c r="N39">
-        <v>35.076999999999998</v>
+        <v>2.75</v>
       </c>
       <c r="O39">
-        <v>34.304000000000002</v>
+        <v>2.875</v>
       </c>
       <c r="P39">
-        <v>33.649000000000001</v>
+        <v>3</v>
       </c>
       <c r="Q39">
-        <v>33.079000000000001</v>
+        <v>3.125</v>
       </c>
       <c r="R39">
-        <v>32.561</v>
+        <v>3.25</v>
       </c>
       <c r="S39">
-        <v>32.061999999999998</v>
+        <v>3.375</v>
       </c>
       <c r="T39">
-        <v>31.547000000000001</v>
+        <v>3.5</v>
       </c>
       <c r="U39">
-        <v>30.984000000000002</v>
+        <v>3.625</v>
       </c>
       <c r="V39">
-        <v>30.373000000000001</v>
+        <v>3.75</v>
       </c>
       <c r="W39">
-        <v>29.745999999999999</v>
+        <v>3.875</v>
       </c>
       <c r="X39">
-        <v>29.113</v>
+        <v>4</v>
       </c>
       <c r="Y39">
-        <v>28.489000000000001</v>
+        <v>4.125</v>
       </c>
       <c r="Z39">
-        <v>27.884</v>
+        <v>4.25</v>
       </c>
       <c r="AA39">
-        <v>27.31</v>
+        <v>4.375</v>
       </c>
       <c r="AB39">
-        <v>26.797999999999998</v>
+        <v>4.5</v>
       </c>
       <c r="AC39">
-        <v>26.350999999999999</v>
+        <v>4.625</v>
       </c>
       <c r="AD39">
-        <v>25.937000000000001</v>
+        <v>4.75</v>
       </c>
       <c r="AE39">
-        <v>25.526</v>
+        <v>4.875</v>
       </c>
       <c r="AF39">
-        <v>25.087</v>
+        <v>5</v>
       </c>
       <c r="AG39">
-        <v>24.59</v>
+        <v>5.125</v>
       </c>
       <c r="AH39">
-        <v>24.004999999999999</v>
+        <v>5.25</v>
       </c>
       <c r="AI39">
-        <v>23.3</v>
+        <v>5.375</v>
       </c>
       <c r="AJ39">
-        <v>22.16</v>
+        <v>5.5</v>
       </c>
       <c r="AK39">
-        <v>21.483000000000001</v>
+        <v>5.625</v>
       </c>
       <c r="AL39">
-        <v>20.917999999999999</v>
+        <v>5.75</v>
       </c>
       <c r="AM39">
-        <v>20.440000000000001</v>
+        <v>5.875</v>
       </c>
       <c r="AN39">
-        <v>20.023</v>
+        <v>6</v>
       </c>
       <c r="AO39">
-        <v>19.64</v>
+        <v>6.125</v>
       </c>
       <c r="AP39">
-        <v>19.265000000000001</v>
+        <v>6.25</v>
       </c>
       <c r="AQ39">
-        <v>18.870999999999999</v>
+        <v>6.375</v>
       </c>
       <c r="AR39">
-        <v>18.465</v>
+        <v>6.5</v>
       </c>
       <c r="AS39">
-        <v>18.071000000000002</v>
+        <v>6.625</v>
       </c>
       <c r="AT39">
-        <v>17.690000000000001</v>
+        <v>6.75</v>
       </c>
       <c r="AU39">
-        <v>17.321999999999999</v>
+        <v>6.875</v>
       </c>
       <c r="AV39">
-        <v>16.969000000000001</v>
+        <v>7</v>
       </c>
       <c r="AW39">
-        <v>16.63</v>
+        <v>7.125</v>
       </c>
       <c r="AX39">
-        <v>16.308</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="40" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>0.75</v>
+        <v>6.8819999999999997</v>
       </c>
       <c r="B40">
-        <v>4.4240000000000004</v>
+        <v>18.625</v>
       </c>
       <c r="C40">
-        <v>7.01</v>
+        <v>26.263999999999999</v>
       </c>
       <c r="D40">
-        <v>13.365</v>
+        <v>34.796999999999997</v>
       </c>
       <c r="E40">
-        <v>13.618</v>
+        <v>35.384</v>
       </c>
       <c r="F40">
-        <v>15.457000000000001</v>
+        <v>36.887999999999998</v>
       </c>
       <c r="G40">
-        <v>17.771999999999998</v>
+        <v>37.512</v>
       </c>
       <c r="H40">
-        <v>11.872999999999999</v>
+        <v>28.463000000000001</v>
       </c>
       <c r="I40">
-        <v>19.634</v>
+        <v>38.103999999999999</v>
       </c>
       <c r="J40">
-        <v>21.734999999999999</v>
+        <v>37.331000000000003</v>
       </c>
       <c r="K40">
-        <v>21.488</v>
+        <v>36.798999999999999</v>
       </c>
       <c r="L40">
-        <v>21.446000000000002</v>
+        <v>37.634</v>
       </c>
       <c r="M40">
-        <v>22.018999999999998</v>
+        <v>36.225999999999999</v>
       </c>
       <c r="N40">
-        <v>22.594000000000001</v>
+        <v>35.076999999999998</v>
       </c>
       <c r="O40">
-        <v>22.568999999999999</v>
+        <v>34.304000000000002</v>
       </c>
       <c r="P40">
-        <v>22.5</v>
+        <v>33.649000000000001</v>
       </c>
       <c r="Q40">
-        <v>22.395</v>
+        <v>33.079000000000001</v>
       </c>
       <c r="R40">
-        <v>22.259</v>
+        <v>32.561</v>
       </c>
       <c r="S40">
-        <v>22.102</v>
+        <v>32.061999999999998</v>
       </c>
       <c r="T40">
-        <v>21.93</v>
+        <v>31.547000000000001</v>
       </c>
       <c r="U40">
-        <v>21.751000000000001</v>
+        <v>30.984000000000002</v>
       </c>
       <c r="V40">
-        <v>21.523</v>
+        <v>30.373000000000001</v>
       </c>
       <c r="W40">
-        <v>21.215</v>
+        <v>29.745999999999999</v>
       </c>
       <c r="X40">
-        <v>20.853000000000002</v>
+        <v>29.113</v>
       </c>
       <c r="Y40">
-        <v>20.463999999999999</v>
+        <v>28.489000000000001</v>
       </c>
       <c r="Z40">
-        <v>20.073</v>
+        <v>27.884</v>
       </c>
       <c r="AA40">
-        <v>19.704999999999998</v>
+        <v>27.31</v>
       </c>
       <c r="AB40">
-        <v>19.318000000000001</v>
+        <v>26.797999999999998</v>
       </c>
       <c r="AC40">
-        <v>18.872</v>
+        <v>26.350999999999999</v>
       </c>
       <c r="AD40">
-        <v>18.402000000000001</v>
+        <v>25.937000000000001</v>
       </c>
       <c r="AE40">
-        <v>17.942</v>
+        <v>25.526</v>
       </c>
       <c r="AF40">
-        <v>17.524999999999999</v>
+        <v>25.087</v>
       </c>
       <c r="AG40">
-        <v>17.184999999999999</v>
+        <v>24.59</v>
       </c>
       <c r="AH40">
-        <v>16.957000000000001</v>
+        <v>24.004999999999999</v>
       </c>
       <c r="AI40">
-        <v>16.873000000000001</v>
+        <v>23.3</v>
       </c>
       <c r="AJ40">
-        <v>21</v>
+        <v>22.16</v>
       </c>
       <c r="AK40">
-        <v>20.975999999999999</v>
+        <v>21.483000000000001</v>
       </c>
       <c r="AL40">
-        <v>20.908999999999999</v>
+        <v>20.917999999999999</v>
       </c>
       <c r="AM40">
-        <v>20.806000000000001</v>
+        <v>20.440000000000001</v>
       </c>
       <c r="AN40">
-        <v>20.672999999999998</v>
+        <v>20.023</v>
       </c>
       <c r="AO40">
-        <v>20.515000000000001</v>
+        <v>19.64</v>
       </c>
       <c r="AP40">
-        <v>20.341000000000001</v>
+        <v>19.265000000000001</v>
       </c>
       <c r="AQ40">
-        <v>20.155999999999999</v>
+        <v>18.870999999999999</v>
       </c>
       <c r="AR40">
-        <v>19.922999999999998</v>
+        <v>18.465</v>
       </c>
       <c r="AS40">
-        <v>19.606999999999999</v>
+        <v>18.071000000000002</v>
       </c>
       <c r="AT40">
-        <v>19.219000000000001</v>
+        <v>17.690000000000001</v>
       </c>
       <c r="AU40">
-        <v>18.77</v>
+        <v>17.321999999999999</v>
       </c>
       <c r="AV40">
-        <v>18.268999999999998</v>
+        <v>16.969000000000001</v>
       </c>
       <c r="AW40">
-        <v>17.728000000000002</v>
+        <v>16.63</v>
       </c>
       <c r="AX40">
-        <v>17.157</v>
+        <v>16.308</v>
       </c>
     </row>
     <row r="41" spans="1:50" x14ac:dyDescent="0.25">
@@ -7285,458 +7285,458 @@
     </row>
     <row r="43" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>1.1111111111111112</v>
+        <v>10</v>
       </c>
       <c r="B43">
-        <v>1.2222222222222223</v>
+        <v>11</v>
       </c>
       <c r="C43">
-        <v>1.3333333333333333</v>
+        <v>12</v>
       </c>
       <c r="D43">
-        <v>1.4444444444444444</v>
+        <v>13</v>
       </c>
       <c r="E43">
-        <v>1.5555555555555556</v>
+        <v>14</v>
       </c>
       <c r="F43">
-        <v>1.6666666666666665</v>
+        <v>15</v>
       </c>
       <c r="G43">
-        <v>1.7777777777777777</v>
+        <v>16</v>
       </c>
       <c r="H43">
-        <v>1.8888888888888888</v>
+        <v>17</v>
       </c>
       <c r="I43">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="J43">
-        <v>2.1111111111111112</v>
+        <v>19</v>
       </c>
       <c r="K43">
-        <v>2.2222222222222223</v>
+        <v>20</v>
       </c>
       <c r="L43">
-        <v>2.333333333333333</v>
+        <v>21</v>
       </c>
       <c r="M43">
-        <v>2.4444444444444446</v>
+        <v>22</v>
       </c>
       <c r="N43">
-        <v>2.5555555555555554</v>
+        <v>23</v>
       </c>
       <c r="O43">
-        <v>2.666666666666667</v>
+        <v>24</v>
       </c>
       <c r="P43">
-        <v>2.7777777777777777</v>
+        <v>25</v>
       </c>
       <c r="Q43">
-        <v>2.8888888888888888</v>
+        <v>26</v>
       </c>
       <c r="R43">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="S43">
-        <v>3.1111111111111112</v>
+        <v>28</v>
       </c>
       <c r="T43">
-        <v>3.2222222222222223</v>
+        <v>29</v>
       </c>
       <c r="U43">
-        <v>3.3333333333333335</v>
+        <v>30</v>
       </c>
       <c r="V43">
-        <v>3.4444444444444446</v>
+        <v>31</v>
       </c>
       <c r="W43">
-        <v>3.5555555555555554</v>
+        <v>32</v>
       </c>
       <c r="X43">
-        <v>3.6666666666666665</v>
+        <v>33</v>
       </c>
       <c r="Y43">
-        <v>3.7777777777777777</v>
+        <v>34</v>
       </c>
       <c r="Z43">
-        <v>3.8888888888888888</v>
+        <v>35</v>
       </c>
       <c r="AA43">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="AB43">
-        <v>4.1111111111111107</v>
+        <v>37</v>
       </c>
       <c r="AC43">
-        <v>4.2222222222222223</v>
+        <v>38</v>
       </c>
       <c r="AD43">
-        <v>4.3333333333333339</v>
+        <v>39</v>
       </c>
       <c r="AE43">
-        <v>4.4444444444444446</v>
+        <v>40</v>
       </c>
       <c r="AF43">
-        <v>4.5555555555555554</v>
+        <v>41</v>
       </c>
       <c r="AG43">
-        <v>4.6666666666666661</v>
+        <v>42</v>
       </c>
       <c r="AH43">
-        <v>4.7777777777777777</v>
+        <v>43</v>
       </c>
       <c r="AI43">
-        <v>4.8888888888888893</v>
+        <v>44</v>
       </c>
       <c r="AJ43">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="AK43">
-        <v>5.1111111111111107</v>
+        <v>46</v>
       </c>
       <c r="AL43">
-        <v>5.2222222222222223</v>
+        <v>47</v>
       </c>
       <c r="AM43">
-        <v>5.333333333333333</v>
+        <v>48</v>
       </c>
       <c r="AN43">
-        <v>5.4444444444444446</v>
+        <v>49</v>
       </c>
       <c r="AO43">
-        <v>5.5555555555555554</v>
+        <v>50</v>
       </c>
       <c r="AP43">
-        <v>5.666666666666667</v>
+        <v>51</v>
       </c>
       <c r="AQ43">
-        <v>5.7777777777777777</v>
+        <v>52</v>
       </c>
       <c r="AR43">
-        <v>5.8888888888888893</v>
+        <v>53</v>
       </c>
       <c r="AS43">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="AT43">
-        <v>6.1111111111111107</v>
+        <v>55</v>
       </c>
       <c r="AU43">
-        <v>6.2222222222222223</v>
+        <v>56</v>
       </c>
       <c r="AV43">
-        <v>6.333333333333333</v>
+        <v>57</v>
       </c>
       <c r="AW43">
-        <v>6.4444444444444446</v>
+        <v>58</v>
       </c>
       <c r="AX43">
-        <v>6.5555555555555554</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>7.024</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="B44">
-        <v>17.890999999999998</v>
+        <v>1.2222222222222223</v>
       </c>
       <c r="C44">
-        <v>20.375</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="D44">
-        <v>31.635000000000002</v>
+        <v>1.4444444444444444</v>
       </c>
       <c r="E44">
-        <v>34.787999999999997</v>
+        <v>1.5555555555555556</v>
       </c>
       <c r="F44">
-        <v>36.567</v>
+        <v>1.6666666666666665</v>
       </c>
       <c r="G44">
-        <v>37.472000000000001</v>
+        <v>1.7777777777777777</v>
       </c>
       <c r="H44">
-        <v>37.548000000000002</v>
+        <v>1.8888888888888888</v>
       </c>
       <c r="I44">
-        <v>30.902999999999999</v>
+        <v>2</v>
       </c>
       <c r="J44">
-        <v>37.173000000000002</v>
+        <v>2.1111111111111112</v>
       </c>
       <c r="K44">
-        <v>36.15</v>
+        <v>2.2222222222222223</v>
       </c>
       <c r="L44">
-        <v>36.21</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="M44">
-        <v>34.792000000000002</v>
+        <v>2.4444444444444446</v>
       </c>
       <c r="N44">
-        <v>34.313000000000002</v>
+        <v>2.5555555555555554</v>
       </c>
       <c r="O44">
-        <v>33.750999999999998</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="P44">
-        <v>33.134999999999998</v>
+        <v>2.7777777777777777</v>
       </c>
       <c r="Q44">
-        <v>32.481999999999999</v>
+        <v>2.8888888888888888</v>
       </c>
       <c r="R44">
-        <v>31.809000000000001</v>
+        <v>3</v>
       </c>
       <c r="S44">
-        <v>31.132999999999999</v>
+        <v>3.1111111111111112</v>
       </c>
       <c r="T44">
-        <v>30.471</v>
+        <v>3.2222222222222223</v>
       </c>
       <c r="U44">
-        <v>29.841000000000001</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="V44">
-        <v>29.234000000000002</v>
+        <v>3.4444444444444446</v>
       </c>
       <c r="W44">
-        <v>28.632999999999999</v>
+        <v>3.5555555555555554</v>
       </c>
       <c r="X44">
-        <v>28.041</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="Y44">
-        <v>27.46</v>
+        <v>3.7777777777777777</v>
       </c>
       <c r="Z44">
-        <v>26.895</v>
+        <v>3.8888888888888888</v>
       </c>
       <c r="AA44">
-        <v>26.349</v>
+        <v>4</v>
       </c>
       <c r="AB44">
-        <v>25.841999999999999</v>
+        <v>4.1111111111111107</v>
       </c>
       <c r="AC44">
-        <v>25.379000000000001</v>
+        <v>4.2222222222222223</v>
       </c>
       <c r="AD44">
-        <v>24.940999999999999</v>
+        <v>4.3333333333333339</v>
       </c>
       <c r="AE44">
-        <v>24.506</v>
+        <v>4.4444444444444446</v>
       </c>
       <c r="AF44">
-        <v>24.056000000000001</v>
+        <v>4.5555555555555554</v>
       </c>
       <c r="AG44">
-        <v>23.568999999999999</v>
+        <v>4.6666666666666661</v>
       </c>
       <c r="AH44">
-        <v>23.027000000000001</v>
+        <v>4.7777777777777777</v>
       </c>
       <c r="AI44">
-        <v>22.408000000000001</v>
+        <v>4.8888888888888893</v>
       </c>
       <c r="AJ44">
-        <v>21.574999999999999</v>
+        <v>5</v>
       </c>
       <c r="AK44">
-        <v>21.05</v>
+        <v>5.1111111111111107</v>
       </c>
       <c r="AL44">
-        <v>20.632999999999999</v>
+        <v>5.2222222222222223</v>
       </c>
       <c r="AM44">
-        <v>20.268000000000001</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="AN44">
-        <v>19.899000000000001</v>
+        <v>5.4444444444444446</v>
       </c>
       <c r="AO44">
-        <v>19.535</v>
+        <v>5.5555555555555554</v>
       </c>
       <c r="AP44">
-        <v>19.187000000000001</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="AQ44">
-        <v>18.800999999999998</v>
+        <v>5.7777777777777777</v>
       </c>
       <c r="AR44">
-        <v>18.311</v>
+        <v>5.8888888888888893</v>
       </c>
       <c r="AS44">
-        <v>17.77</v>
+        <v>6</v>
       </c>
       <c r="AT44">
-        <v>17.302</v>
+        <v>6.1111111111111107</v>
       </c>
       <c r="AU44">
-        <v>16.925000000000001</v>
+        <v>6.2222222222222223</v>
       </c>
       <c r="AV44">
-        <v>16.581</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="AW44">
-        <v>16.283000000000001</v>
+        <v>6.4444444444444446</v>
       </c>
       <c r="AX44">
-        <v>16.042000000000002</v>
+        <v>6.5555555555555554</v>
       </c>
     </row>
     <row r="45" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>0.72399999999999998</v>
+        <v>7.024</v>
       </c>
       <c r="B45">
-        <v>3.3959999999999999</v>
+        <v>17.890999999999998</v>
       </c>
       <c r="C45">
-        <v>1.93</v>
+        <v>20.375</v>
       </c>
       <c r="D45">
-        <v>9.3190000000000008</v>
+        <v>31.635000000000002</v>
       </c>
       <c r="E45">
-        <v>12.391999999999999</v>
+        <v>34.787999999999997</v>
       </c>
       <c r="F45">
-        <v>14.154</v>
+        <v>36.567</v>
       </c>
       <c r="G45">
-        <v>15.906000000000001</v>
+        <v>37.472000000000001</v>
       </c>
       <c r="H45">
-        <v>17.152999999999999</v>
+        <v>37.548000000000002</v>
       </c>
       <c r="I45">
-        <v>13.397</v>
+        <v>30.902999999999999</v>
       </c>
       <c r="J45">
-        <v>18.827999999999999</v>
+        <v>37.173000000000002</v>
       </c>
       <c r="K45">
-        <v>20.684999999999999</v>
+        <v>36.15</v>
       </c>
       <c r="L45">
-        <v>19.873000000000001</v>
+        <v>36.21</v>
       </c>
       <c r="M45">
-        <v>19.885999999999999</v>
+        <v>34.792000000000002</v>
       </c>
       <c r="N45">
-        <v>20.763999999999999</v>
+        <v>34.313000000000002</v>
       </c>
       <c r="O45">
-        <v>21.225000000000001</v>
+        <v>33.750999999999998</v>
       </c>
       <c r="P45">
-        <v>21.638000000000002</v>
+        <v>33.134999999999998</v>
       </c>
       <c r="Q45">
-        <v>21.995000000000001</v>
+        <v>32.481999999999999</v>
       </c>
       <c r="R45">
-        <v>22.286999999999999</v>
+        <v>31.809000000000001</v>
       </c>
       <c r="S45">
-        <v>22.506</v>
+        <v>31.132999999999999</v>
       </c>
       <c r="T45">
-        <v>22.643000000000001</v>
+        <v>30.471</v>
       </c>
       <c r="U45">
-        <v>22.690999999999999</v>
+        <v>29.841000000000001</v>
       </c>
       <c r="V45">
-        <v>22.218</v>
+        <v>29.234000000000002</v>
       </c>
       <c r="W45">
-        <v>21.029</v>
+        <v>28.632999999999999</v>
       </c>
       <c r="X45">
-        <v>19.47</v>
+        <v>28.041</v>
       </c>
       <c r="Y45">
-        <v>17.888000000000002</v>
+        <v>27.46</v>
       </c>
       <c r="Z45">
-        <v>16.63</v>
+        <v>26.895</v>
       </c>
       <c r="AA45">
-        <v>16.041</v>
+        <v>26.349</v>
       </c>
       <c r="AB45">
-        <v>15.926</v>
+        <v>25.841999999999999</v>
       </c>
       <c r="AC45">
-        <v>15.851000000000001</v>
+        <v>25.379000000000001</v>
       </c>
       <c r="AD45">
-        <v>15.801</v>
+        <v>24.940999999999999</v>
       </c>
       <c r="AE45">
-        <v>15.763999999999999</v>
+        <v>24.506</v>
       </c>
       <c r="AF45">
-        <v>15.727</v>
+        <v>24.056000000000001</v>
       </c>
       <c r="AG45">
-        <v>15.675000000000001</v>
+        <v>23.568999999999999</v>
       </c>
       <c r="AH45">
-        <v>15.596</v>
+        <v>23.027000000000001</v>
       </c>
       <c r="AI45">
-        <v>15.476000000000001</v>
+        <v>22.408000000000001</v>
       </c>
       <c r="AJ45">
-        <v>15.1</v>
+        <v>21.574999999999999</v>
       </c>
       <c r="AK45">
-        <v>14.776999999999999</v>
+        <v>21.05</v>
       </c>
       <c r="AL45">
-        <v>14.481999999999999</v>
+        <v>20.632999999999999</v>
       </c>
       <c r="AM45">
-        <v>14.176</v>
+        <v>20.268000000000001</v>
       </c>
       <c r="AN45">
-        <v>13.815</v>
+        <v>19.899000000000001</v>
       </c>
       <c r="AO45">
-        <v>13.278</v>
+        <v>19.535</v>
       </c>
       <c r="AP45">
-        <v>12.662000000000001</v>
+        <v>19.187000000000001</v>
       </c>
       <c r="AQ45">
-        <v>12.252000000000001</v>
+        <v>18.800999999999998</v>
       </c>
       <c r="AR45">
-        <v>12.086</v>
+        <v>18.311</v>
       </c>
       <c r="AS45">
-        <v>11.973000000000001</v>
+        <v>17.77</v>
       </c>
       <c r="AT45">
-        <v>11.852</v>
+        <v>17.302</v>
       </c>
       <c r="AU45">
-        <v>11.702</v>
+        <v>16.925000000000001</v>
       </c>
       <c r="AV45">
-        <v>11.544</v>
+        <v>16.581</v>
       </c>
       <c r="AW45">
-        <v>11.377000000000001</v>
+        <v>16.283000000000001</v>
       </c>
       <c r="AX45">
-        <v>11.202</v>
+        <v>16.042000000000002</v>
       </c>
     </row>
     <row r="46" spans="1:50" x14ac:dyDescent="0.25">
@@ -8045,458 +8045,458 @@
     </row>
     <row r="48" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>1.1000000000000001</v>
+        <v>11</v>
       </c>
       <c r="B48">
-        <v>1.2</v>
+        <v>12</v>
       </c>
       <c r="C48">
-        <v>1.3</v>
+        <v>13</v>
       </c>
       <c r="D48">
-        <v>1.4</v>
+        <v>14</v>
       </c>
       <c r="E48">
-        <v>1.5</v>
+        <v>15</v>
       </c>
       <c r="F48">
-        <v>1.6</v>
+        <v>16</v>
       </c>
       <c r="G48">
-        <v>1.7</v>
+        <v>17</v>
       </c>
       <c r="H48">
-        <v>1.8</v>
+        <v>18</v>
       </c>
       <c r="I48">
-        <v>1.9</v>
+        <v>19</v>
       </c>
       <c r="J48">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="K48">
-        <v>2.1</v>
+        <v>21</v>
       </c>
       <c r="L48">
-        <v>2.2000000000000002</v>
+        <v>22</v>
       </c>
       <c r="M48">
-        <v>2.2999999999999998</v>
+        <v>23</v>
       </c>
       <c r="N48">
-        <v>2.4</v>
+        <v>24</v>
       </c>
       <c r="O48">
-        <v>2.5</v>
+        <v>25</v>
       </c>
       <c r="P48">
-        <v>2.6</v>
+        <v>26</v>
       </c>
       <c r="Q48">
-        <v>2.7</v>
+        <v>27</v>
       </c>
       <c r="R48">
-        <v>2.8</v>
+        <v>28</v>
       </c>
       <c r="S48">
-        <v>2.9</v>
+        <v>29</v>
       </c>
       <c r="T48">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="U48">
-        <v>3.1</v>
+        <v>31</v>
       </c>
       <c r="V48">
-        <v>3.2</v>
+        <v>32</v>
       </c>
       <c r="W48">
-        <v>3.3</v>
+        <v>33</v>
       </c>
       <c r="X48">
-        <v>3.4</v>
+        <v>34</v>
       </c>
       <c r="Y48">
-        <v>3.5</v>
+        <v>35</v>
       </c>
       <c r="Z48">
-        <v>3.6</v>
+        <v>36</v>
       </c>
       <c r="AA48">
-        <v>3.7</v>
+        <v>37</v>
       </c>
       <c r="AB48">
-        <v>3.8</v>
+        <v>38</v>
       </c>
       <c r="AC48">
-        <v>3.9</v>
+        <v>39</v>
       </c>
       <c r="AD48">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="AE48">
-        <v>4.0999999999999996</v>
+        <v>41</v>
       </c>
       <c r="AF48">
-        <v>4.2</v>
+        <v>42</v>
       </c>
       <c r="AG48">
-        <v>4.3</v>
+        <v>43</v>
       </c>
       <c r="AH48">
-        <v>4.4000000000000004</v>
+        <v>44</v>
       </c>
       <c r="AI48">
-        <v>4.5</v>
+        <v>45</v>
       </c>
       <c r="AJ48">
-        <v>4.5999999999999996</v>
+        <v>46</v>
       </c>
       <c r="AK48">
-        <v>4.7</v>
+        <v>47</v>
       </c>
       <c r="AL48">
-        <v>4.8</v>
+        <v>48</v>
       </c>
       <c r="AM48">
-        <v>4.9000000000000004</v>
+        <v>49</v>
       </c>
       <c r="AN48">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="AO48">
-        <v>5.0999999999999996</v>
+        <v>51</v>
       </c>
       <c r="AP48">
-        <v>5.2</v>
+        <v>52</v>
       </c>
       <c r="AQ48">
-        <v>5.3</v>
+        <v>53</v>
       </c>
       <c r="AR48">
-        <v>5.4</v>
+        <v>54</v>
       </c>
       <c r="AS48">
-        <v>5.5</v>
+        <v>55</v>
       </c>
       <c r="AT48">
-        <v>5.6</v>
+        <v>56</v>
       </c>
       <c r="AU48">
-        <v>5.7</v>
+        <v>57</v>
       </c>
       <c r="AV48">
-        <v>5.8</v>
+        <v>58</v>
       </c>
       <c r="AW48">
-        <v>5.9</v>
+        <v>59</v>
       </c>
       <c r="AX48">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>7.1959999999999997</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B49">
-        <v>15.981999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="C49">
-        <v>26.283999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="D49">
-        <v>32.046999999999997</v>
+        <v>1.4</v>
       </c>
       <c r="E49">
-        <v>37.659999999999997</v>
+        <v>1.5</v>
       </c>
       <c r="F49">
-        <v>34.978999999999999</v>
+        <v>1.6</v>
       </c>
       <c r="G49">
-        <v>36.915999999999997</v>
+        <v>1.7</v>
       </c>
       <c r="H49">
-        <v>37.012</v>
+        <v>1.8</v>
       </c>
       <c r="I49">
-        <v>36.354999999999997</v>
+        <v>1.9</v>
       </c>
       <c r="J49">
-        <v>32.981000000000002</v>
+        <v>2</v>
       </c>
       <c r="K49">
-        <v>35.247999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="L49">
-        <v>35.186999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M49">
-        <v>34.131</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N49">
-        <v>33.435000000000002</v>
+        <v>2.4</v>
       </c>
       <c r="O49">
-        <v>32.741</v>
+        <v>2.5</v>
       </c>
       <c r="P49">
-        <v>32.042999999999999</v>
+        <v>2.6</v>
       </c>
       <c r="Q49">
-        <v>31.344999999999999</v>
+        <v>2.7</v>
       </c>
       <c r="R49">
-        <v>30.654</v>
+        <v>2.8</v>
       </c>
       <c r="S49">
-        <v>29.975000000000001</v>
+        <v>2.9</v>
       </c>
       <c r="T49">
-        <v>29.312999999999999</v>
+        <v>3</v>
       </c>
       <c r="U49">
-        <v>28.673999999999999</v>
+        <v>3.1</v>
       </c>
       <c r="V49">
-        <v>28.053999999999998</v>
+        <v>3.2</v>
       </c>
       <c r="W49">
-        <v>27.446000000000002</v>
+        <v>3.3</v>
       </c>
       <c r="X49">
-        <v>26.853000000000002</v>
+        <v>3.4</v>
       </c>
       <c r="Y49">
-        <v>26.277000000000001</v>
+        <v>3.5</v>
       </c>
       <c r="Z49">
-        <v>25.72</v>
+        <v>3.6</v>
       </c>
       <c r="AA49">
-        <v>25.184000000000001</v>
+        <v>3.7</v>
       </c>
       <c r="AB49">
-        <v>24.696999999999999</v>
+        <v>3.8</v>
       </c>
       <c r="AC49">
-        <v>24.265999999999998</v>
+        <v>3.9</v>
       </c>
       <c r="AD49">
-        <v>23.866</v>
+        <v>4</v>
       </c>
       <c r="AE49">
-        <v>23.47</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AF49">
-        <v>23.050999999999998</v>
+        <v>4.2</v>
       </c>
       <c r="AG49">
-        <v>22.584</v>
+        <v>4.3</v>
       </c>
       <c r="AH49">
-        <v>22.042000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AI49">
-        <v>21.398</v>
+        <v>4.5</v>
       </c>
       <c r="AJ49">
-        <v>20.413</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AK49">
-        <v>19.763999999999999</v>
+        <v>4.7</v>
       </c>
       <c r="AL49">
-        <v>19.218</v>
+        <v>4.8</v>
       </c>
       <c r="AM49">
-        <v>18.783000000000001</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AN49">
-        <v>18.466000000000001</v>
+        <v>5</v>
       </c>
       <c r="AO49">
-        <v>18.279</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="AP49">
-        <v>18.143000000000001</v>
+        <v>5.2</v>
       </c>
       <c r="AQ49">
-        <v>17.931000000000001</v>
+        <v>5.3</v>
       </c>
       <c r="AR49">
-        <v>17.300999999999998</v>
+        <v>5.4</v>
       </c>
       <c r="AS49">
-        <v>16.332999999999998</v>
+        <v>5.5</v>
       </c>
       <c r="AT49">
-        <v>15.535</v>
+        <v>5.6</v>
       </c>
       <c r="AU49">
-        <v>15.010999999999999</v>
+        <v>5.7</v>
       </c>
       <c r="AV49">
-        <v>14.547000000000001</v>
+        <v>5.8</v>
       </c>
       <c r="AW49">
-        <v>14.176</v>
+        <v>5.9</v>
       </c>
       <c r="AX49">
-        <v>13.928000000000001</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>0.61799999999999999</v>
+        <v>7.1959999999999997</v>
       </c>
       <c r="B50">
-        <v>1.143</v>
+        <v>15.981999999999999</v>
       </c>
       <c r="C50">
-        <v>6.0449999999999999</v>
+        <v>26.283999999999999</v>
       </c>
       <c r="D50">
-        <v>8.7490000000000006</v>
+        <v>32.046999999999997</v>
       </c>
       <c r="E50">
-        <v>13.711</v>
+        <v>37.659999999999997</v>
       </c>
       <c r="F50">
-        <v>11.441000000000001</v>
+        <v>34.978999999999999</v>
       </c>
       <c r="G50">
-        <v>15.009</v>
+        <v>36.915999999999997</v>
       </c>
       <c r="H50">
-        <v>16.712</v>
+        <v>37.012</v>
       </c>
       <c r="I50">
-        <v>17.091999999999999</v>
+        <v>36.354999999999997</v>
       </c>
       <c r="J50">
-        <v>14.356</v>
+        <v>32.981000000000002</v>
       </c>
       <c r="K50">
-        <v>19.288</v>
+        <v>35.247999999999998</v>
       </c>
       <c r="L50">
-        <v>18.48</v>
+        <v>35.186999999999998</v>
       </c>
       <c r="M50">
-        <v>18.963000000000001</v>
+        <v>34.131</v>
       </c>
       <c r="N50">
-        <v>19.484000000000002</v>
+        <v>33.435000000000002</v>
       </c>
       <c r="O50">
-        <v>19.459</v>
+        <v>32.741</v>
       </c>
       <c r="P50">
-        <v>19.388999999999999</v>
+        <v>32.042999999999999</v>
       </c>
       <c r="Q50">
-        <v>19.282</v>
+        <v>31.344999999999999</v>
       </c>
       <c r="R50">
-        <v>19.146000000000001</v>
+        <v>30.654</v>
       </c>
       <c r="S50">
-        <v>18.989999999999998</v>
+        <v>29.975000000000001</v>
       </c>
       <c r="T50">
-        <v>18.821999999999999</v>
+        <v>29.312999999999999</v>
       </c>
       <c r="U50">
-        <v>18.649000000000001</v>
+        <v>28.673999999999999</v>
       </c>
       <c r="V50">
-        <v>18.440999999999999</v>
+        <v>28.053999999999998</v>
       </c>
       <c r="W50">
-        <v>18.173999999999999</v>
+        <v>27.446000000000002</v>
       </c>
       <c r="X50">
-        <v>17.864999999999998</v>
+        <v>26.853000000000002</v>
       </c>
       <c r="Y50">
-        <v>17.533000000000001</v>
+        <v>26.277000000000001</v>
       </c>
       <c r="Z50">
-        <v>17.196999999999999</v>
+        <v>25.72</v>
       </c>
       <c r="AA50">
-        <v>16.875</v>
+        <v>25.184000000000001</v>
       </c>
       <c r="AB50">
-        <v>16.553000000000001</v>
+        <v>24.696999999999999</v>
       </c>
       <c r="AC50">
-        <v>16.21</v>
+        <v>24.265999999999998</v>
       </c>
       <c r="AD50">
-        <v>15.856999999999999</v>
+        <v>23.866</v>
       </c>
       <c r="AE50">
-        <v>15.503</v>
+        <v>23.47</v>
       </c>
       <c r="AF50">
-        <v>15.157999999999999</v>
+        <v>23.050999999999998</v>
       </c>
       <c r="AG50">
-        <v>14.831</v>
+        <v>22.584</v>
       </c>
       <c r="AH50">
-        <v>14.532</v>
+        <v>22.042000000000002</v>
       </c>
       <c r="AI50">
-        <v>14.27</v>
+        <v>21.398</v>
       </c>
       <c r="AJ50">
-        <v>14.061999999999999</v>
+        <v>20.413</v>
       </c>
       <c r="AK50">
-        <v>14.667</v>
+        <v>19.763999999999999</v>
       </c>
       <c r="AL50">
-        <v>15.999000000000001</v>
+        <v>19.218</v>
       </c>
       <c r="AM50">
-        <v>17.331</v>
+        <v>18.783000000000001</v>
       </c>
       <c r="AN50">
-        <v>17.936</v>
+        <v>18.466000000000001</v>
       </c>
       <c r="AO50">
-        <v>16.225999999999999</v>
+        <v>18.279</v>
       </c>
       <c r="AP50">
-        <v>13.052</v>
+        <v>18.143000000000001</v>
       </c>
       <c r="AQ50">
-        <v>11.342000000000001</v>
+        <v>17.931000000000001</v>
       </c>
       <c r="AR50">
-        <v>12.526</v>
+        <v>17.300999999999998</v>
       </c>
       <c r="AS50">
-        <v>14.725</v>
+        <v>16.332999999999998</v>
       </c>
       <c r="AT50">
-        <v>15.909000000000001</v>
+        <v>15.535</v>
       </c>
       <c r="AU50">
-        <v>15.349</v>
+        <v>15.010999999999999</v>
       </c>
       <c r="AV50">
-        <v>13.686</v>
+        <v>14.547000000000001</v>
       </c>
       <c r="AW50">
-        <v>10.945</v>
+        <v>14.176</v>
       </c>
       <c r="AX50">
-        <v>7.1529999999999996</v>
+        <v>13.928000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:50" x14ac:dyDescent="0.25">

</xml_diff>